<commit_message>
added sigup and verify lead details tests for lms
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="login" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="lmsUserData" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Flag</t>
   </si>
@@ -52,6 +53,60 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>target_year</t>
+  </si>
+  <si>
+    <t>leadType</t>
+  </si>
+  <si>
+    <t>campaignUrl</t>
+  </si>
+  <si>
+    <t>baseUrl</t>
+  </si>
+  <si>
+    <t>test user</t>
+  </si>
+  <si>
+    <t>testuser@plancess.com</t>
+  </si>
+  <si>
+    <t>9000000969</t>
+  </si>
+  <si>
+    <t>mumbai</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>NR Lead</t>
+  </si>
+  <si>
+    <t>Chhagan</t>
+  </si>
+  <si>
+    <t>http://pages.plancessjee.com/campaign-study-material-vcm1</t>
+  </si>
+  <si>
+    <t>http://pages.plancessjee.com/</t>
+  </si>
+  <si>
+    <t>R Lead</t>
   </si>
 </sst>
 </file>
@@ -61,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -86,6 +141,20 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -133,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -146,6 +215,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -155,6 +232,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF2A00FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -165,8 +302,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -262,4 +399,155 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="50.6122448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.8826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A3" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="testuser@plancess.com"/>
+    <hyperlink ref="J2" r:id="rId2" display="http://pages.plancessjee.com/campaign-study-material-vcm1"/>
+    <hyperlink ref="C3" r:id="rId3" display="testuser@plancess.com"/>
+    <hyperlink ref="J3" r:id="rId4" display="http://pages.plancessjee.com/campaign-study-material-vcm1"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
addded create campaign test and takeTest test
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,19 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="login" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="lmsUserData" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="lmsUserData" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Campaign" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="assessment" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
   <si>
     <t>Flag</t>
   </si>
@@ -46,7 +47,22 @@
     <t>No</t>
   </si>
   <si>
-    <t>flag</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>target_year</t>
+  </si>
+  <si>
+    <t>leadType</t>
   </si>
   <si>
     <t>username</t>
@@ -55,24 +71,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>mobile</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>target_year</t>
-  </si>
-  <si>
-    <t>leadType</t>
-  </si>
-  <si>
     <t>campaignUrl</t>
   </si>
   <si>
@@ -107,14 +105,150 @@
   </si>
   <si>
     <t>R Lead</t>
+  </si>
+  <si>
+    <t>campaignName</t>
+  </si>
+  <si>
+    <t>campaignType</t>
+  </si>
+  <si>
+    <t>channels</t>
+  </si>
+  <si>
+    <t>vendors</t>
+  </si>
+  <si>
+    <t>expectedLeads</t>
+  </si>
+  <si>
+    <t>totalBudget</t>
+  </si>
+  <si>
+    <t>startDate</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>welcomeEmail</t>
+  </si>
+  <si>
+    <t>welcomeSMS</t>
+  </si>
+  <si>
+    <t>allocate_demo</t>
+  </si>
+  <si>
+    <t>mailerContent</t>
+  </si>
+  <si>
+    <t>campaignDescription</t>
+  </si>
+  <si>
+    <t>targetAudiences</t>
+  </si>
+  <si>
+    <t>http://192.168.1.9:810/</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin@#</t>
+  </si>
+  <si>
+    <t>Automation Test Campaign 150904</t>
+  </si>
+  <si>
+    <t>Emailer</t>
+  </si>
+  <si>
+    <t>Google,Facebook</t>
+  </si>
+  <si>
+    <t>Shiksha,Plancess</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>15/09/2015</t>
+  </si>
+  <si>
+    <t>30/09/2015</t>
+  </si>
+  <si>
+    <t>Welcome Email</t>
+  </si>
+  <si>
+    <t>Welcome SMS</t>
+  </si>
+  <si>
+    <t>Some mail content</t>
+  </si>
+  <si>
+    <t>This is a test campaign</t>
+  </si>
+  <si>
+    <t>Automation Test Campaign 150902</t>
+  </si>
+  <si>
+    <t>Creative</t>
+  </si>
+  <si>
+    <t>Email,SMS</t>
+  </si>
+  <si>
+    <t>Plancess,Shiksha</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>20/09/2015</t>
+  </si>
+  <si>
+    <t>29/09/2015</t>
+  </si>
+  <si>
+    <t>FREEDOM Offer - Thank You</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>answerChoices</t>
+  </si>
+  <si>
+    <t>http://dev.plancess.com/ui/#/</t>
+  </si>
+  <si>
+    <t>webuser10@plancess.com</t>
+  </si>
+  <si>
+    <t>P@ssw0rd</t>
+  </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -202,7 +336,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -220,6 +354,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -303,7 +445,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -368,48 +510,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K3"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -429,69 +533,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,34 +603,34 @@
         <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -550,4 +654,303 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:R3"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3520408163265"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="50.6122448979592"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.8826530612245"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.0765306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.7142857142857"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.4642857142857"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A3" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://192.168.1.9:810/"/>
+    <hyperlink ref="B3" r:id="rId2" display="http://192.168.1.9:810/"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/#/"/>
+    <hyperlink ref="C2" r:id="rId2" display="webuser10@plancess.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added takeTest positive scenario
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -11,14 +11,15 @@
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="lmsUserData" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Campaign" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="assessment" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="assessment_valid" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="assessment_no_test" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
   <si>
     <t>Flag</t>
   </si>
@@ -44,39 +45,51 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>WebUser</t>
+  </si>
+  <si>
+    <t>testuser11@plancess.com</t>
+  </si>
+  <si>
+    <t>P@ssw0rd</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>target_year</t>
+  </si>
+  <si>
+    <t>leadType</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>campaignUrl</t>
+  </si>
+  <si>
+    <t>baseUrl</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>mobile</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>target_year</t>
-  </si>
-  <si>
-    <t>leadType</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>campaignUrl</t>
-  </si>
-  <si>
-    <t>baseUrl</t>
-  </si>
-  <si>
     <t>test user</t>
   </si>
   <si>
@@ -227,19 +240,34 @@
     <t>answerChoices</t>
   </si>
   <si>
-    <t>http://dev.plancess.com/ui/#/</t>
-  </si>
-  <si>
-    <t>webuser10@plancess.com</t>
-  </si>
-  <si>
-    <t>P@ssw0rd</t>
-  </si>
-  <si>
-    <t>math</t>
+    <t>http://dev.plancess.com/ui/app/#/</t>
+  </si>
+  <si>
+    <t>testuser1@plancess.com</t>
+  </si>
+  <si>
+    <t>chemistry</t>
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>testuser2@plancess.com</t>
+  </si>
+  <si>
+    <t>physics</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>testuser3@plancess.com</t>
+  </si>
+  <si>
+    <t>maths</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -250,7 +278,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -292,6 +320,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -336,7 +370,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -363,6 +397,14 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -442,15 +484,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.1020408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9897959183673"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
@@ -482,19 +526,37 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>9876543210</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A3" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="testuser11@plancess.com"/>
+    <hyperlink ref="F2" r:id="rId2" display="P@ssw0rd"/>
+    <hyperlink ref="G2" r:id="rId3" display="P@ssw0rd"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -533,69 +595,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -603,34 +665,34 @@
         <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -694,55 +756,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -750,105 +812,105 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="O3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -877,18 +939,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3520408163265"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
@@ -898,52 +961,205 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>73</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A4" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/#/"/>
-    <hyperlink ref="C2" r:id="rId2" display="webuser10@plancess.com"/>
+    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
     <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+    <hyperlink ref="B3" r:id="rId4" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C3" r:id="rId5" display="testuser2@plancess.com"/>
+    <hyperlink ref="D3" r:id="rId6" display="P@ssw0rd"/>
+    <hyperlink ref="B4" r:id="rId7" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C4" r:id="rId8" display="testuser3@plancess.com"/>
+    <hyperlink ref="D4" r:id="rId9" display="P@ssw0rd"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A3" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+    <hyperlink ref="B3" r:id="rId4" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C3" r:id="rId5" display="testuser2@plancess.com"/>
+    <hyperlink ref="D3" r:id="rId6" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added tests for login from landing page
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="801" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,13 +13,18 @@
     <sheet name="Campaign" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="assessment_valid" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="assessment_no_test" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="nonExistingEmails" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="invalidPasswords" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="loginWithValidEmailPassword" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="signupInvalidEmails" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="signUpvalidEmailPasswords" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="119">
   <si>
     <t>Flag</t>
   </si>
@@ -240,43 +245,152 @@
     <t>answerChoices</t>
   </si>
   <si>
+    <t>timeRequired</t>
+  </si>
+  <si>
+    <t>totalQuestions</t>
+  </si>
+  <si>
     <t>http://dev.plancess.com/ui/app/#/</t>
   </si>
   <si>
     <t>testuser1@plancess.com</t>
   </si>
   <si>
+    <t>physics</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>00: 30: 00</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>testuser2@plancess.com</t>
+  </si>
+  <si>
+    <t>maths</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>testuser4@plancess.com</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>testuser5@plancess.com</t>
+  </si>
+  <si>
+    <t>testuser6@plancess.com</t>
+  </si>
+  <si>
     <t>chemistry</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>testuser2@plancess.com</t>
-  </si>
-  <si>
-    <t>physics</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>testuser3@plancess.com</t>
-  </si>
-  <si>
-    <t>maths</t>
-  </si>
-  <si>
-    <t>c</t>
+    <t>nonexistingemail@plancess.com</t>
+  </si>
+  <si>
+    <t>InvalidPassword</t>
+  </si>
+  <si>
+    <t>http://dev.plancess.com/ui/app/</t>
+  </si>
+  <si>
+    <t>confirm_password</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>web.test.firstname.lastname1</t>
+  </si>
+  <si>
+    <t>@plancess.com</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>9876543210</t>
+  </si>
+  <si>
+    <t>webtestuser2</t>
+  </si>
+  <si>
+    <t>webtestuser3</t>
+  </si>
+  <si>
+    <t>@plancess-edu.com</t>
+  </si>
+  <si>
+    <t>firstname+lastname+web+test4</t>
+  </si>
+  <si>
+    <t>firstname.lastnamewebtest5</t>
+  </si>
+  <si>
+    <t>@123.123.123.123</t>
+  </si>
+  <si>
+    <t>firstname.lastnamewebtest6</t>
+  </si>
+  <si>
+    <t>@[123.123.123.123]</t>
+  </si>
+  <si>
+    <t>"firstname.lastnamewebtest7</t>
+  </si>
+  <si>
+    <t>"@plancess.com</t>
+  </si>
+  <si>
+    <t>1234567890webtest8</t>
+  </si>
+  <si>
+    <t>firstname.lastnamewebtest39</t>
+  </si>
+  <si>
+    <t>@plancess.name</t>
+  </si>
+  <si>
+    <t>____@webtest10</t>
+  </si>
+  <si>
+    <t>plancess.com</t>
+  </si>
+  <si>
+    <t>emailwebtest11</t>
+  </si>
+  <si>
+    <t>@plancess.co.in</t>
+  </si>
+  <si>
+    <t>firstname-lastnamewebtest12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -370,7 +484,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -399,12 +513,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -567,6 +685,514 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A13" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+    <hyperlink ref="E2" r:id="rId4" display="P@ssw0rd"/>
+    <hyperlink ref="B3" r:id="rId5" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C3" r:id="rId6" display="testuser1@plancess.com"/>
+    <hyperlink ref="D3" r:id="rId7" display="P@ssw0rd"/>
+    <hyperlink ref="E3" r:id="rId8" display="P@ssw0rd"/>
+    <hyperlink ref="B4" r:id="rId9" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C4" r:id="rId10" display="testuser1@plancess.com"/>
+    <hyperlink ref="D4" r:id="rId11" display="P@ssw0rd"/>
+    <hyperlink ref="E4" r:id="rId12" display="P@ssw0rd"/>
+    <hyperlink ref="B5" r:id="rId13" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C5" r:id="rId14" display="testuser1@plancess.com"/>
+    <hyperlink ref="D5" r:id="rId15" display="P@ssw0rd"/>
+    <hyperlink ref="E5" r:id="rId16" display="P@ssw0rd"/>
+    <hyperlink ref="B6" r:id="rId17" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C6" r:id="rId18" display="testuser1@plancess.com"/>
+    <hyperlink ref="D6" r:id="rId19" display="P@ssw0rd"/>
+    <hyperlink ref="E6" r:id="rId20" display="P@ssw0rd"/>
+    <hyperlink ref="B7" r:id="rId21" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C7" r:id="rId22" display="testuser1@plancess.com"/>
+    <hyperlink ref="D7" r:id="rId23" display="P@ssw0rd"/>
+    <hyperlink ref="E7" r:id="rId24" display="P@ssw0rd"/>
+    <hyperlink ref="B8" r:id="rId25" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C8" r:id="rId26" display="testuser1@plancess.com"/>
+    <hyperlink ref="D8" r:id="rId27" display="P@ssw0rd"/>
+    <hyperlink ref="E8" r:id="rId28" display="P@ssw0rd"/>
+    <hyperlink ref="B9" r:id="rId29" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C9" r:id="rId30" display="testuser1@plancess.com"/>
+    <hyperlink ref="D9" r:id="rId31" display="P@ssw0rd"/>
+    <hyperlink ref="E9" r:id="rId32" display="P@ssw0rd"/>
+    <hyperlink ref="B10" r:id="rId33" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C10" r:id="rId34" display="testuser1@plancess.com"/>
+    <hyperlink ref="D10" r:id="rId35" display="P@ssw0rd"/>
+    <hyperlink ref="E10" r:id="rId36" display="P@ssw0rd"/>
+    <hyperlink ref="B11" r:id="rId37" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C11" r:id="rId38" display="testuser1@plancess.com"/>
+    <hyperlink ref="D11" r:id="rId39" display="P@ssw0rd"/>
+    <hyperlink ref="E11" r:id="rId40" display="P@ssw0rd"/>
+    <hyperlink ref="B12" r:id="rId41" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C12" r:id="rId42" display="testuser1@plancess.com"/>
+    <hyperlink ref="D12" r:id="rId43" display="P@ssw0rd"/>
+    <hyperlink ref="E12" r:id="rId44" display="P@ssw0rd"/>
+    <hyperlink ref="B13" r:id="rId45" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C13" r:id="rId46" display="testuser1@plancess.com"/>
+    <hyperlink ref="D13" r:id="rId47" display="P@ssw0rd"/>
+    <hyperlink ref="E13" r:id="rId48" display="P@ssw0rd"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -939,10 +1565,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -953,7 +1579,9 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1020408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,45 +1603,63 @@
       <c r="F1" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>79</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,38 +1667,101 @@
         <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>80</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A4" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A6" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
-    <hyperlink ref="B3" r:id="rId4" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C3" r:id="rId5" display="testuser2@plancess.com"/>
-    <hyperlink ref="D3" r:id="rId6" display="P@ssw0rd"/>
-    <hyperlink ref="B4" r:id="rId7" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C4" r:id="rId8" display="testuser3@plancess.com"/>
-    <hyperlink ref="D4" r:id="rId9" display="P@ssw0rd"/>
+    <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
+    <hyperlink ref="B3" r:id="rId3" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C3" r:id="rId4" display="testuser2@plancess.com"/>
+    <hyperlink ref="D3" r:id="rId5" display="P@ssw0rd"/>
+    <hyperlink ref="B4" r:id="rId6" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C4" r:id="rId7" display="testuser4@plancess.com"/>
+    <hyperlink ref="D4" r:id="rId8" display="P@ssw0rd"/>
+    <hyperlink ref="B5" r:id="rId9" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C5" r:id="rId10" display="testuser5@plancess.com"/>
+    <hyperlink ref="D5" r:id="rId11" display="P@ssw0rd"/>
+    <hyperlink ref="B6" r:id="rId12" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C6" r:id="rId13" display="testuser6@plancess.com"/>
+    <hyperlink ref="D6" r:id="rId14" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1111,19 +1820,19 @@
         <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,19 +1840,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="F3" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1169,4 +1878,298 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C2" r:id="rId2" display="nonexistingemail@plancess.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="testuser1@plancess.com"/>
+    <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
dashboard tests in progress
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="801" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="801" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,13 +18,14 @@
     <sheet name="loginWithValidEmailPassword" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="signupInvalidEmails" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="signUpvalidEmailPasswords" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="dashboard" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="119">
   <si>
     <t>Flag</t>
   </si>
@@ -392,7 +393,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -434,12 +435,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -484,7 +479,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -519,10 +514,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1193,6 +1184,79 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="testuser1@plancess.com"/>
+    <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -2034,8 +2098,8 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2069,7 +2133,7 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C2" s="8" t="s">

</xml_diff>

<commit_message>
added create assessment test
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="801" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="801" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,13 +19,14 @@
     <sheet name="signupInvalidEmails" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="signUpvalidEmailPasswords" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="dashboard" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="createAssessment" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="127">
   <si>
     <t>Flag</t>
   </si>
@@ -382,6 +383,30 @@
   </si>
   <si>
     <t>firstname-lastnamewebtest12</t>
+  </si>
+  <si>
+    <t>ExamType</t>
+  </si>
+  <si>
+    <t>Test Duration</t>
+  </si>
+  <si>
+    <t>Difficulty Level</t>
+  </si>
+  <si>
+    <t>http://dev.plancess.com/ui/</t>
+  </si>
+  <si>
+    <t>Physics&gt;Mechanics&gt;Motion in a Straight Line</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>45 mins</t>
+  </si>
+  <si>
+    <t>Easy</t>
   </si>
 </sst>
 </file>
@@ -591,6 +616,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G2"/>
@@ -679,6 +705,7 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:13"/>
@@ -1187,12 +1214,13 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1257,9 +1285,108 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.7244897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
+    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K3"/>
@@ -1411,6 +1538,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:R3"/>
@@ -1627,6 +1755,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H6"/>
@@ -1840,6 +1969,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F3"/>
@@ -1947,6 +2077,7 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:2"/>
@@ -2021,6 +2152,7 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:2"/>
@@ -2094,6 +2226,7 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:2"/>
@@ -2167,6 +2300,7 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:2"/>

</xml_diff>

<commit_message>
added login with facebook test
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="801" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="801" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,13 +19,15 @@
     <sheet name="signupInvalidEmails" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="signUpvalidEmailPasswords" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="dashboard" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="loginWithFacebook" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="loginWithGoogle" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="128">
   <si>
     <t>Flag</t>
   </si>
@@ -382,6 +384,33 @@
   </si>
   <si>
     <t>firstname-lastnamewebtest12</t>
+  </si>
+  <si>
+    <t>fbEmail</t>
+  </si>
+  <si>
+    <t>fbPassword</t>
+  </si>
+  <si>
+    <t>http://dev.plancess.com/ui/</t>
+  </si>
+  <si>
+    <t>9167360969</t>
+  </si>
+  <si>
+    <t>Cl#12345</t>
+  </si>
+  <si>
+    <t>googleEmail</t>
+  </si>
+  <si>
+    <t>googlePassword</t>
+  </si>
+  <si>
+    <t>chhaganmathuriya@gmail.com</t>
+  </si>
+  <si>
+    <t>harshitlodhi</t>
   </si>
 </sst>
 </file>
@@ -1191,8 +1220,8 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1246,6 +1275,151 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="testuser1@plancess.com"/>
     <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
+    <hyperlink ref="C2" r:id="rId2" display="chhaganmathuriya@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added create assessment test with parameterization
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="144">
   <si>
     <t>Flag</t>
   </si>
@@ -388,25 +388,76 @@
     <t>ExamType</t>
   </si>
   <si>
-    <t>Test Duration</t>
-  </si>
-  <si>
-    <t>Difficulty Level</t>
+    <t>TestDuration</t>
+  </si>
+  <si>
+    <t>DifficultyLevel</t>
   </si>
   <si>
     <t>http://dev.plancess.com/ui/</t>
   </si>
   <si>
-    <t>Physics&gt;Mechanics&gt;Motion in a Straight Line</t>
+    <t>Physics&gt;Mechanics&gt;Motion In A Plane</t>
   </si>
   <si>
     <t>Main</t>
   </si>
   <si>
+    <t>30 mins</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Physics&gt;Optics&gt;Wave Optics,Chemistry&gt;Organic Chemistry&gt;Alkanes,Mathematics&gt;Vectors &amp; 3D&gt;3D Geometry</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
     <t>45 mins</t>
   </si>
   <si>
-    <t>Easy</t>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>00: 45: 00</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Mathematics&gt;Calculas&gt;Differential Equations,Mathematics&gt;Calculas&gt;Definite Integration,Mathematics&gt;Calculas&gt;Indefinite Integration,Mathematics&gt;Calculas&gt;Relations and Functions</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>Mathematics&gt;Calculas&gt;Differential Equations,Mathematics&gt;Calculas&gt;Definite Integration,Mathematics&gt;Calculas&gt;Indefinite Integration,Mathematics&gt;Calculas&gt;Relations and Functions,Mathematics&gt;Algebra&gt;Basic Mathematics,Mathematics&gt;Algebra&gt; Binomial Theorem,Mathematics&gt;Algebra&gt;Complex Number,Mathematics&gt;Algebra&gt;Determinants</t>
+  </si>
+  <si>
+    <t>60 mins</t>
+  </si>
+  <si>
+    <t>Extreme</t>
+  </si>
+  <si>
+    <t>00: 60: 00</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Physics&gt;Waves and Thermodynamics&gt;</t>
+  </si>
+  <si>
+    <t>Physics&gt;Waves and Thermodynamics&gt;,Chemistry&gt;Inorganic Chemistry&gt;</t>
+  </si>
+  <si>
+    <t>Physics&gt;Modern Physics&gt;Modern Physics,Chemistry&gt;Physical Chemistry&gt;Atomic Structure,Mathematics&gt;Trigonometry&gt;Solutions of Triangle</t>
   </si>
 </sst>
 </file>
@@ -1291,18 +1342,19 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.7244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="123.515306122449"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.780612244898"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.9795918367347"/>
@@ -1334,10 +1386,19 @@
       <c r="H1" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>122</v>
@@ -1360,10 +1421,229 @@
       <c r="H2" s="0" t="s">
         <v>126</v>
       </c>
+      <c r="I2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>140</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A8" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1372,6 +1652,24 @@
     <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
     <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
     <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+    <hyperlink ref="B3" r:id="rId4" display="http://dev.plancess.com/ui/"/>
+    <hyperlink ref="C3" r:id="rId5" display="testuser1@plancess.com"/>
+    <hyperlink ref="D3" r:id="rId6" display="P@ssw0rd"/>
+    <hyperlink ref="B4" r:id="rId7" display="http://dev.plancess.com/ui/"/>
+    <hyperlink ref="C4" r:id="rId8" display="testuser1@plancess.com"/>
+    <hyperlink ref="D4" r:id="rId9" display="P@ssw0rd"/>
+    <hyperlink ref="B5" r:id="rId10" display="http://dev.plancess.com/ui/"/>
+    <hyperlink ref="C5" r:id="rId11" display="testuser1@plancess.com"/>
+    <hyperlink ref="D5" r:id="rId12" display="P@ssw0rd"/>
+    <hyperlink ref="B6" r:id="rId13" display="http://dev.plancess.com/ui/"/>
+    <hyperlink ref="C6" r:id="rId14" display="testuser1@plancess.com"/>
+    <hyperlink ref="D6" r:id="rId15" display="P@ssw0rd"/>
+    <hyperlink ref="B7" r:id="rId16" display="http://dev.plancess.com/ui/"/>
+    <hyperlink ref="C7" r:id="rId17" display="testuser1@plancess.com"/>
+    <hyperlink ref="D7" r:id="rId18" display="P@ssw0rd"/>
+    <hyperlink ref="B8" r:id="rId19" display="http://dev.plancess.com/ui/"/>
+    <hyperlink ref="C8" r:id="rId20" display="testuser1@plancess.com"/>
+    <hyperlink ref="D8" r:id="rId21" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1761,7 +2059,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2158,7 +2456,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
updated social login tests
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="801" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="277" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,12 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="127">
   <si>
     <t>Flag</t>
   </si>
   <si>
-    <t>FirstName</t>
+    <t>firstName</t>
   </si>
   <si>
     <t>LastName</t>
@@ -314,9 +314,6 @@
     <t>domain</t>
   </si>
   <si>
-    <t>firstName</t>
-  </si>
-  <si>
     <t>lastName</t>
   </si>
   <si>
@@ -398,7 +395,7 @@
     <t>9167360969</t>
   </si>
   <si>
-    <t>Cl#12345</t>
+    <t>Cl$12345</t>
   </si>
   <si>
     <t>googleEmail</t>
@@ -407,10 +404,10 @@
     <t>googlePassword</t>
   </si>
   <si>
-    <t>chhaganmathuriya@gmail.com</t>
-  </si>
-  <si>
-    <t>harshitlodhi</t>
+    <t>chhaganlal.m@plancess.com</t>
+  </si>
+  <si>
+    <t>Pla@12345</t>
   </si>
 </sst>
 </file>
@@ -453,14 +450,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF2A00FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF2A00FF"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -517,11 +514,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -541,7 +538,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -624,8 +621,8 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -641,7 +638,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -661,7 +658,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -670,16 +667,16 @@
       <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>9876543210</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -750,10 +747,10 @@
         <v>94</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -763,387 +760,387 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>98</v>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J3" s="0" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>98</v>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J6" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>110</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J8" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J8" s="0" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>98</v>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="0" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I10" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J10" s="0" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>115</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I11" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J11" s="0" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I12" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J12" s="0" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>98</v>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I13" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1252,16 +1249,16 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>92</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1294,7 +1291,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1314,10 +1311,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -1325,17 +1322,17 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1365,8 +1362,8 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1386,10 +1383,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -1397,17 +1394,17 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>121</v>
+      <c r="B2" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1419,7 +1416,8 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C2" r:id="rId2" display="chhaganmathuriya@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="chhaganlal.m@plancess.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="Pla@12345"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1490,13 +1488,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -1517,21 +1515,21 @@
       <c r="I2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -1552,10 +1550,10 @@
       <c r="I3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1672,10 +1670,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -1725,10 +1723,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -1849,16 +1847,16 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -1875,16 +1873,16 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
@@ -1901,16 +1899,16 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
@@ -1927,16 +1925,16 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -1953,16 +1951,16 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
@@ -2054,16 +2052,16 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -2074,16 +2072,16 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
@@ -2157,16 +2155,16 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2231,16 +2229,16 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2304,16 +2302,16 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>92</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2377,16 +2375,16 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
to run login test on jenkins
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="149">
   <si>
     <t>Flag</t>
   </si>
@@ -393,22 +393,16 @@
     <t>http://dev.plancess.com/ui/</t>
   </si>
   <si>
-    <t>9167360969</t>
-  </si>
-  <si>
-    <t>Cl$12345</t>
+    <t>chhaganlal.m@plancess.com</t>
+  </si>
+  <si>
+    <t>Pla@12345</t>
   </si>
   <si>
     <t>googleEmail</t>
   </si>
   <si>
     <t>googlePassword</t>
-  </si>
-  <si>
-    <t>chhaganlal.m@plancess.com</t>
-  </si>
-  <si>
-    <t>Pla@12345</t>
   </si>
   <si>
     <t>ExamType</t>
@@ -695,7 +689,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -783,7 +777,7 @@
   <dimension ref="1:13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1291,7 +1285,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1363,8 +1357,8 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1417,6 +1411,8 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
+    <hyperlink ref="C2" r:id="rId2" display="chhaganlal.m@plancess.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="Pla@12345"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1436,7 +1432,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1474,10 +1470,10 @@
         <v>120</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1509,8 +1505,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1543,13 +1539,13 @@
         <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>72</v>
@@ -1575,16 +1571,16 @@
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>133</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>78</v>
@@ -1593,7 +1589,7 @@
         <v>79</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,25 +1606,25 @@
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>138</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1645,25 +1641,25 @@
         <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>86</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,25 +1676,25 @@
         <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>143</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>145</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>86</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1715,25 +1711,25 @@
         <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>133</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>78</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,25 +1746,25 @@
         <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>138</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1785,25 +1781,25 @@
         <v>11</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>86</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1854,7 +1850,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2005,7 +2001,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2221,7 +2217,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2434,7 +2430,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2541,7 +2537,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2615,7 +2611,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2688,7 +2684,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2761,7 +2757,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
to run selenium tests with headless firefox
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="150">
   <si>
     <t>Flag</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>googlePassword</t>
+  </si>
+  <si>
+    <t>9167360969</t>
   </si>
   <si>
     <t>ExamType</t>
@@ -1357,7 +1360,7 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1431,8 +1434,8 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1457,6 +1460,9 @@
       <c r="D1" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -1474,6 +1480,9 @@
       </c>
       <c r="D2" s="4" t="s">
         <v>122</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1539,13 +1548,13 @@
         <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>72</v>
@@ -1571,16 +1580,16 @@
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>78</v>
@@ -1589,7 +1598,7 @@
         <v>79</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1606,25 +1615,25 @@
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1641,25 +1650,25 @@
         <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>86</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1676,25 +1685,25 @@
         <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>86</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,25 +1720,25 @@
         <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>78</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,25 +1755,25 @@
         <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1781,25 +1790,25 @@
         <v>11</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>86</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
signup with email verification complete, dashboard content test
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="144">
   <si>
     <t>Flag</t>
   </si>
@@ -309,6 +309,9 @@
     <t>http://dev.plancess.com/ui/app/</t>
   </si>
   <si>
+    <t>cl100@mailinator.com</t>
+  </si>
+  <si>
     <t>confirm_password</t>
   </si>
   <si>
@@ -348,16 +351,13 @@
     <t>firstname.ltest6</t>
   </si>
   <si>
-    <t>"firstname.l7</t>
+    <t>firstname.l7</t>
   </si>
   <si>
     <t>1234567890w8</t>
   </si>
   <si>
     <t>firstname.ltest39</t>
-  </si>
-  <si>
-    <t>____@webtest10</t>
   </si>
   <si>
     <t>emailwebtest11</t>
@@ -759,10 +759,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:13"/>
+  <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -787,7 +787,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>19</v>
@@ -796,13 +796,13 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -819,7 +819,7 @@
         <v>75</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -828,19 +828,19 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,7 +851,7 @@
         <v>75</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -860,19 +860,19 @@
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -883,7 +883,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
@@ -892,19 +892,19 @@
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,7 +915,7 @@
         <v>75</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
@@ -924,19 +924,19 @@
         <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,7 +947,7 @@
         <v>75</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
@@ -956,19 +956,19 @@
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,7 +979,7 @@
         <v>75</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -988,19 +988,19 @@
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,7 +1011,7 @@
         <v>75</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
@@ -1020,19 +1020,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>11</v>
@@ -1052,19 +1052,19 @@
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,7 +1075,7 @@
         <v>75</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>11</v>
@@ -1084,19 +1084,19 @@
         <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1107,7 +1107,7 @@
         <v>75</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>11</v>
@@ -1116,19 +1116,19 @@
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,7 +1139,7 @@
         <v>75</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>11</v>
@@ -1148,56 +1148,24 @@
         <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A13" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A12" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1236,9 +1204,6 @@
     <hyperlink ref="B12" r:id="rId31" location="/" display="http://dev.plancess.com/ui/app/#/"/>
     <hyperlink ref="D12" r:id="rId32" display="P@ssw0rd"/>
     <hyperlink ref="E12" r:id="rId33" display="P@ssw0rd"/>
-    <hyperlink ref="B13" r:id="rId34" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D13" r:id="rId35" display="P@ssw0rd"/>
-    <hyperlink ref="E13" r:id="rId36" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1405,7 +1370,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2662,8 +2627,8 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2701,7 +2666,7 @@
         <v>92</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -2715,7 +2680,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="testuser1@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="cl100@mailinator.com"/>
     <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added dashboard content tests
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -366,6 +366,9 @@
     <t>Firstname-ltest12</t>
   </si>
   <si>
+    <t>chhaganlal.m@plancess.com</t>
+  </si>
+  <si>
     <t>fbEmail</t>
   </si>
   <si>
@@ -373,9 +376,6 @@
   </si>
   <si>
     <t>http://dev.plancess.com/ui/</t>
-  </si>
-  <si>
-    <t>chhaganlal.m@plancess.com</t>
   </si>
   <si>
     <t>Pla@12345</t>
@@ -1222,8 +1222,8 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1261,7 +1261,7 @@
         <v>92</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -1275,7 +1275,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="testuser1@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="chhaganlal.m@plancess.com"/>
     <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1316,10 +1316,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -1331,10 +1331,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>116</v>
@@ -1408,10 +1408,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>116</v>
@@ -1506,7 +1506,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>76</v>
@@ -1541,7 +1541,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>76</v>
@@ -1576,7 +1576,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>76</v>
@@ -1611,7 +1611,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>76</v>
@@ -1646,7 +1646,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>76</v>
@@ -1681,7 +1681,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>76</v>
@@ -1716,7 +1716,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>76</v>
@@ -2627,7 +2627,7 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added take subject test
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -297,6 +297,9 @@
     <t>testuser6@plancess.com</t>
   </si>
   <si>
+    <t>chhaganlal.m@plancess.com</t>
+  </si>
+  <si>
     <t>chemistry</t>
   </si>
   <si>
@@ -364,9 +367,6 @@
   </si>
   <si>
     <t>Firstname-ltest12</t>
-  </si>
-  <si>
-    <t>chhaganlal.m@plancess.com</t>
   </si>
   <si>
     <t>fbEmail</t>
@@ -674,7 +674,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="2" sqref="C3 D12 D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -762,7 +762,7 @@
   <dimension ref="1:12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="2" sqref="C3 D12 F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -787,7 +787,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>19</v>
@@ -796,13 +796,13 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -819,7 +819,7 @@
         <v>75</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -828,19 +828,19 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,7 +851,7 @@
         <v>75</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -860,19 +860,19 @@
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -883,7 +883,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
@@ -892,19 +892,19 @@
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,7 +915,7 @@
         <v>75</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
@@ -924,19 +924,19 @@
         <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,7 +947,7 @@
         <v>75</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
@@ -956,19 +956,19 @@
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,7 +979,7 @@
         <v>75</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -988,19 +988,19 @@
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,7 +1011,7 @@
         <v>75</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
@@ -1020,19 +1020,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>11</v>
@@ -1052,19 +1052,19 @@
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,7 +1075,7 @@
         <v>75</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>11</v>
@@ -1084,19 +1084,19 @@
         <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1107,7 +1107,7 @@
         <v>75</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>11</v>
@@ -1116,19 +1116,19 @@
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,7 +1139,7 @@
         <v>75</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>11</v>
@@ -1148,19 +1148,19 @@
         <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1222,8 +1222,8 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3 D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1258,10 +1258,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -1296,7 +1296,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3 D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1334,7 +1334,7 @@
         <v>115</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>116</v>
@@ -1370,7 +1370,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="2" sqref="C3 D12 F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1411,7 +1411,7 @@
         <v>115</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>116</v>
@@ -1450,7 +1450,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="C3 D12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1794,7 +1794,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="2" sqref="C3 D12 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1945,7 +1945,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="C3 D12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2161,7 +2161,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="2" sqref="C3 D12 H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2373,8 +2373,8 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="C3 D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2416,13 +2416,13 @@
         <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>78</v>
@@ -2435,8 +2435,8 @@
       <c r="B3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>81</v>
+      <c r="C3" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -2457,10 +2457,10 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="chhaganlal.m@plancess.com"/>
     <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
     <hyperlink ref="B3" r:id="rId4" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C3" r:id="rId5" display="testuser2@plancess.com"/>
+    <hyperlink ref="C3" r:id="rId5" display="chhaganlal.m@plancess.com"/>
     <hyperlink ref="D3" r:id="rId6" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2481,7 +2481,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="2" sqref="C3 D12 B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2519,7 +2519,7 @@
         <v>75</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -2555,7 +2555,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="2" sqref="C3 D12 C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2596,7 +2596,7 @@
         <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2628,7 +2628,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3 D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2663,10 +2663,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -2701,7 +2701,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="2" sqref="C3 D12 B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
updated create assessment test
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="145">
   <si>
     <t>Flag</t>
   </si>
@@ -312,6 +312,9 @@
     <t>cl100@mailinator.com</t>
   </si>
   <si>
+    <t>stestuser1@mailinator.com</t>
+  </si>
+  <si>
     <t>confirm_password</t>
   </si>
   <si>
@@ -447,7 +450,7 @@
     <t>Extreme</t>
   </si>
   <si>
-    <t>00: 60: 00</t>
+    <t>01: 00: 00</t>
   </si>
   <si>
     <t>30</t>
@@ -787,7 +790,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>19</v>
@@ -796,13 +799,13 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -819,7 +822,7 @@
         <v>75</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -828,19 +831,19 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,7 +854,7 @@
         <v>75</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -860,19 +863,19 @@
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -883,7 +886,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
@@ -892,19 +895,19 @@
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,7 +918,7 @@
         <v>75</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
@@ -924,19 +927,19 @@
         <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,7 +950,7 @@
         <v>75</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
@@ -956,19 +959,19 @@
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,7 +982,7 @@
         <v>75</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -988,19 +991,19 @@
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,7 +1014,7 @@
         <v>75</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
@@ -1020,19 +1023,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1043,7 +1046,7 @@
         <v>75</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>11</v>
@@ -1052,19 +1055,19 @@
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,7 +1078,7 @@
         <v>75</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>11</v>
@@ -1084,19 +1087,19 @@
         <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1107,7 +1110,7 @@
         <v>75</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>11</v>
@@ -1116,19 +1119,19 @@
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,7 +1142,7 @@
         <v>75</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>11</v>
@@ -1148,19 +1151,19 @@
         <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1222,7 +1225,7 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1261,7 +1264,7 @@
         <v>92</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -1316,10 +1319,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -1331,13 +1334,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1390,10 +1393,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
@@ -1408,16 +1411,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1449,8 +1452,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1483,13 +1486,13 @@
         <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>72</v>
@@ -1506,25 +1509,25 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>78</v>
@@ -1533,7 +1536,7 @@
         <v>79</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1541,34 +1544,34 @@
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,34 +1579,34 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>86</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1611,34 +1614,34 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>86</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1646,34 +1649,34 @@
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>78</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1681,34 +1684,34 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1716,34 +1719,34 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>86</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1755,25 +1758,25 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
     <hyperlink ref="B3" r:id="rId4" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C3" r:id="rId5" display="testuser1@plancess.com"/>
+    <hyperlink ref="C3" r:id="rId5" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D3" r:id="rId6" display="P@ssw0rd"/>
     <hyperlink ref="B4" r:id="rId7" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C4" r:id="rId8" display="testuser1@plancess.com"/>
+    <hyperlink ref="C4" r:id="rId8" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D4" r:id="rId9" display="P@ssw0rd"/>
     <hyperlink ref="B5" r:id="rId10" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C5" r:id="rId11" display="testuser1@plancess.com"/>
+    <hyperlink ref="C5" r:id="rId11" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D5" r:id="rId12" display="P@ssw0rd"/>
     <hyperlink ref="B6" r:id="rId13" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C6" r:id="rId14" display="testuser1@plancess.com"/>
+    <hyperlink ref="C6" r:id="rId14" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D6" r:id="rId15" display="P@ssw0rd"/>
     <hyperlink ref="B7" r:id="rId16" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C7" r:id="rId17" display="testuser1@plancess.com"/>
+    <hyperlink ref="C7" r:id="rId17" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D7" r:id="rId18" display="P@ssw0rd"/>
     <hyperlink ref="B8" r:id="rId19" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C8" r:id="rId20" display="testuser1@plancess.com"/>
+    <hyperlink ref="C8" r:id="rId20" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D8" r:id="rId21" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2160,7 +2163,7 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -2701,7 +2704,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2739,7 +2742,7 @@
         <v>75</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -2754,7 +2757,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
updated take assessment steps
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="138">
   <si>
     <t>Flag</t>
   </si>
@@ -258,159 +258,147 @@
     <t>http://dev.plancess.com/ui/app/#/</t>
   </si>
   <si>
+    <t>chhaganlal.m@plancess.com</t>
+  </si>
+  <si>
+    <t>chemistry</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>01: 00: 00</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>physics</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>nonexistingemail@plancess.com</t>
+  </si>
+  <si>
     <t>testuser1@plancess.com</t>
   </si>
   <si>
-    <t>physics</t>
-  </si>
-  <si>
-    <t>a</t>
+    <t>InvalidPassword</t>
+  </si>
+  <si>
+    <t>http://dev.plancess.com/ui/app/</t>
+  </si>
+  <si>
+    <t>cl100@mailinator.com</t>
+  </si>
+  <si>
+    <t>confirm_password</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>testuser1@mailinator.com</t>
+  </si>
+  <si>
+    <t>web.test.f.l1</t>
+  </si>
+  <si>
+    <t>@mailinator.com</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>9876543210</t>
+  </si>
+  <si>
+    <t>webtestuser2</t>
+  </si>
+  <si>
+    <t>webtestuser3</t>
+  </si>
+  <si>
+    <t>firstname+ltest4</t>
+  </si>
+  <si>
+    <t>firstname.ltest5</t>
+  </si>
+  <si>
+    <t>firstname.ltest6</t>
+  </si>
+  <si>
+    <t>firstname.l7</t>
+  </si>
+  <si>
+    <t>1234567890w8</t>
+  </si>
+  <si>
+    <t>firstname.ltest39</t>
+  </si>
+  <si>
+    <t>emailwebtest11</t>
+  </si>
+  <si>
+    <t>Firstname-ltest12</t>
+  </si>
+  <si>
+    <t>fbEmail</t>
+  </si>
+  <si>
+    <t>fbPassword</t>
+  </si>
+  <si>
+    <t>http://dev.plancess.com/ui/</t>
+  </si>
+  <si>
+    <t>Pla@12345</t>
+  </si>
+  <si>
+    <t>googleEmail</t>
+  </si>
+  <si>
+    <t>googlePassword</t>
+  </si>
+  <si>
+    <t>9167360969</t>
+  </si>
+  <si>
+    <t>ExamType</t>
+  </si>
+  <si>
+    <t>TestDuration</t>
+  </si>
+  <si>
+    <t>DifficultyLevel</t>
+  </si>
+  <si>
+    <t>stestuser1@mailinator.com</t>
+  </si>
+  <si>
+    <t>Physics&gt;Mechanics&gt;Motion In A Plane</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>30 mins</t>
+  </si>
+  <si>
+    <t>Easy</t>
   </si>
   <si>
     <t>00: 30: 00</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>testuser2@plancess.com</t>
-  </si>
-  <si>
-    <t>maths</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>testuser4@plancess.com</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>testuser5@plancess.com</t>
-  </si>
-  <si>
-    <t>testuser6@plancess.com</t>
-  </si>
-  <si>
-    <t>chhaganlal.m@plancess.com</t>
-  </si>
-  <si>
-    <t>chemistry</t>
-  </si>
-  <si>
-    <t>nonexistingemail@plancess.com</t>
-  </si>
-  <si>
-    <t>InvalidPassword</t>
-  </si>
-  <si>
-    <t>http://dev.plancess.com/ui/app/</t>
-  </si>
-  <si>
-    <t>cl100@mailinator.com</t>
-  </si>
-  <si>
-    <t>confirm_password</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>testuser1@mailinator.com</t>
-  </si>
-  <si>
-    <t>web.test.f.l1</t>
-  </si>
-  <si>
-    <t>@mailinator.com</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>9876543210</t>
-  </si>
-  <si>
-    <t>webtestuser2</t>
-  </si>
-  <si>
-    <t>webtestuser3</t>
-  </si>
-  <si>
-    <t>firstname+ltest4</t>
-  </si>
-  <si>
-    <t>firstname.ltest5</t>
-  </si>
-  <si>
-    <t>firstname.ltest6</t>
-  </si>
-  <si>
-    <t>firstname.l7</t>
-  </si>
-  <si>
-    <t>1234567890w8</t>
-  </si>
-  <si>
-    <t>firstname.ltest39</t>
-  </si>
-  <si>
-    <t>emailwebtest11</t>
-  </si>
-  <si>
-    <t>Firstname-ltest12</t>
-  </si>
-  <si>
-    <t>fbEmail</t>
-  </si>
-  <si>
-    <t>fbPassword</t>
-  </si>
-  <si>
-    <t>http://dev.plancess.com/ui/</t>
-  </si>
-  <si>
-    <t>Pla@12345</t>
-  </si>
-  <si>
-    <t>googleEmail</t>
-  </si>
-  <si>
-    <t>googlePassword</t>
-  </si>
-  <si>
-    <t>9167360969</t>
-  </si>
-  <si>
-    <t>ExamType</t>
-  </si>
-  <si>
-    <t>TestDuration</t>
-  </si>
-  <si>
-    <t>DifficultyLevel</t>
-  </si>
-  <si>
-    <t>Physics&gt;Mechanics&gt;Motion In A Plane</t>
-  </si>
-  <si>
-    <t>Main</t>
-  </si>
-  <si>
-    <t>30 mins</t>
-  </si>
-  <si>
-    <t>Easy</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
@@ -445,12 +433,6 @@
   </si>
   <si>
     <t>Extreme</t>
-  </si>
-  <si>
-    <t>00: 60: 00</t>
-  </si>
-  <si>
-    <t>30</t>
   </si>
   <si>
     <t>Physics&gt;Waves and Thermodynamics&gt;</t>
@@ -586,12 +568,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -674,7 +656,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="2" sqref="C3 D12 D32"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -762,7 +744,7 @@
   <dimension ref="1:12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="2" sqref="C3 D12 F12"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -787,7 +769,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>19</v>
@@ -796,13 +778,13 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -818,8 +800,8 @@
       <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>98</v>
+      <c r="C2" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -828,19 +810,19 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,8 +832,8 @@
       <c r="B3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>98</v>
+      <c r="C3" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -860,19 +842,19 @@
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -882,29 +864,29 @@
       <c r="B4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,8 +896,8 @@
       <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>98</v>
+      <c r="C5" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
@@ -924,19 +906,19 @@
         <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,8 +928,8 @@
       <c r="B6" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>98</v>
+      <c r="C6" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
@@ -956,19 +938,19 @@
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,8 +960,8 @@
       <c r="B7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>98</v>
+      <c r="C7" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -988,19 +970,19 @@
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,8 +992,8 @@
       <c r="B8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>98</v>
+      <c r="C8" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
@@ -1020,19 +1002,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1042,8 +1024,8 @@
       <c r="B9" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>98</v>
+      <c r="C9" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>11</v>
@@ -1052,19 +1034,19 @@
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1074,8 +1056,8 @@
       <c r="B10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>98</v>
+      <c r="C10" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>11</v>
@@ -1084,19 +1066,19 @@
         <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,8 +1088,8 @@
       <c r="B11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>98</v>
+      <c r="C11" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>11</v>
@@ -1116,19 +1098,19 @@
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1138,8 +1120,8 @@
       <c r="B12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>98</v>
+      <c r="C12" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>11</v>
@@ -1148,19 +1130,19 @@
         <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1205,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3 D12"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1258,10 +1240,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -1296,7 +1278,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3 D12"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1316,10 +1298,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -1331,13 +1313,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>89</v>
+        <v>109</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1370,7 +1352,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="2" sqref="C3 D12 F14"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1390,10 +1372,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
@@ -1408,16 +1390,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>89</v>
+        <v>109</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1449,8 +1431,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="C3 D12 A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1483,13 +1465,13 @@
         <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>72</v>
@@ -1506,34 +1488,34 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1541,34 +1523,34 @@
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>132</v>
+      <c r="J3" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,34 +1558,34 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>132</v>
+        <v>78</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1611,34 +1593,34 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>139</v>
+        <v>78</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1646,34 +1628,34 @@
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>132</v>
+        <v>81</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1681,34 +1663,34 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>139</v>
+      <c r="J7" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1716,34 +1698,34 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>139</v>
+        <v>78</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1755,25 +1737,25 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
     <hyperlink ref="B3" r:id="rId4" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C3" r:id="rId5" display="testuser1@plancess.com"/>
+    <hyperlink ref="C3" r:id="rId5" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D3" r:id="rId6" display="P@ssw0rd"/>
     <hyperlink ref="B4" r:id="rId7" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C4" r:id="rId8" display="testuser1@plancess.com"/>
+    <hyperlink ref="C4" r:id="rId8" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D4" r:id="rId9" display="P@ssw0rd"/>
     <hyperlink ref="B5" r:id="rId10" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C5" r:id="rId11" display="testuser1@plancess.com"/>
+    <hyperlink ref="C5" r:id="rId11" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D5" r:id="rId12" display="P@ssw0rd"/>
     <hyperlink ref="B6" r:id="rId13" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C6" r:id="rId14" display="testuser1@plancess.com"/>
+    <hyperlink ref="C6" r:id="rId14" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D6" r:id="rId15" display="P@ssw0rd"/>
     <hyperlink ref="B7" r:id="rId16" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C7" r:id="rId17" display="testuser1@plancess.com"/>
+    <hyperlink ref="C7" r:id="rId17" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D7" r:id="rId18" display="P@ssw0rd"/>
     <hyperlink ref="B8" r:id="rId19" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C8" r:id="rId20" display="testuser1@plancess.com"/>
+    <hyperlink ref="C8" r:id="rId20" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D8" r:id="rId21" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1794,7 +1776,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="2" sqref="C3 D12 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1945,7 +1927,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="C3 D12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2158,10 +2140,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="2" sqref="C3 D12 H7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2205,12 +2187,12 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -2222,139 +2204,24 @@
       <c r="F2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="0" t="s">
         <v>79</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
-    <hyperlink ref="B3" r:id="rId3" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C3" r:id="rId4" display="testuser2@plancess.com"/>
-    <hyperlink ref="D3" r:id="rId5" display="P@ssw0rd"/>
-    <hyperlink ref="B4" r:id="rId6" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C4" r:id="rId7" display="testuser4@plancess.com"/>
-    <hyperlink ref="D4" r:id="rId8" display="P@ssw0rd"/>
-    <hyperlink ref="B5" r:id="rId9" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C5" r:id="rId10" display="testuser5@plancess.com"/>
-    <hyperlink ref="D5" r:id="rId11" display="P@ssw0rd"/>
-    <hyperlink ref="B6" r:id="rId12" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C6" r:id="rId13" display="testuser6@plancess.com"/>
-    <hyperlink ref="D6" r:id="rId14" display="P@ssw0rd"/>
+    <hyperlink ref="C2" r:id="rId2" display="chhaganlal.m@plancess.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2373,8 +2240,8 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="C3 D12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2416,16 +2283,16 @@
         <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2436,13 +2303,13 @@
         <v>75</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>83</v>
@@ -2481,7 +2348,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="2" sqref="C3 D12 B18"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2518,8 +2385,8 @@
       <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>91</v>
+      <c r="C2" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -2555,7 +2422,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="2" sqref="C3 D12 C18"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2592,11 +2459,11 @@
       <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>76</v>
+      <c r="C2" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2628,7 +2495,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3 D12"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2663,10 +2530,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -2701,7 +2568,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="2" sqref="C3 D12 B19"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2738,8 +2605,8 @@
       <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>76</v>
+      <c r="C2" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
updated take test scenario
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="138">
   <si>
     <t>Flag</t>
   </si>
@@ -258,159 +258,144 @@
     <t>http://dev.plancess.com/ui/app/#/</t>
   </si>
   <si>
+    <t>chhaganlal.m@plancess.com</t>
+  </si>
+  <si>
+    <t>chemistry</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>01: 00: 00</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>physics</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>nonexistingemail@plancess.com</t>
+  </si>
+  <si>
     <t>testuser1@plancess.com</t>
   </si>
   <si>
-    <t>physics</t>
-  </si>
-  <si>
-    <t>a</t>
+    <t>InvalidPassword</t>
+  </si>
+  <si>
+    <t>http://dev.plancess.com/ui/app/</t>
+  </si>
+  <si>
+    <t>cl100@mailinator.com</t>
+  </si>
+  <si>
+    <t>confirm_password</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>testuser1@mailinator.com</t>
+  </si>
+  <si>
+    <t>web.test.f.l1</t>
+  </si>
+  <si>
+    <t>@mailinator.com</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>9876543210</t>
+  </si>
+  <si>
+    <t>webtestuser2</t>
+  </si>
+  <si>
+    <t>webtestuser3</t>
+  </si>
+  <si>
+    <t>firstname+ltest4</t>
+  </si>
+  <si>
+    <t>firstname.ltest5</t>
+  </si>
+  <si>
+    <t>firstname.ltest6</t>
+  </si>
+  <si>
+    <t>firstname.l7</t>
+  </si>
+  <si>
+    <t>1234567890w8</t>
+  </si>
+  <si>
+    <t>firstname.ltest39</t>
+  </si>
+  <si>
+    <t>emailwebtest11</t>
+  </si>
+  <si>
+    <t>Firstname-ltest12</t>
+  </si>
+  <si>
+    <t>fbEmail</t>
+  </si>
+  <si>
+    <t>fbPassword</t>
+  </si>
+  <si>
+    <t>http://dev.plancess.com/ui/</t>
+  </si>
+  <si>
+    <t>Pla@12345</t>
+  </si>
+  <si>
+    <t>googleEmail</t>
+  </si>
+  <si>
+    <t>googlePassword</t>
+  </si>
+  <si>
+    <t>9167360969</t>
+  </si>
+  <si>
+    <t>ExamType</t>
+  </si>
+  <si>
+    <t>TestDuration</t>
+  </si>
+  <si>
+    <t>DifficultyLevel</t>
+  </si>
+  <si>
+    <t>Physics&gt;Mechanics&gt;Motion In A Plane</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>30 mins</t>
+  </si>
+  <si>
+    <t>Easy</t>
   </si>
   <si>
     <t>00: 30: 00</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>testuser2@plancess.com</t>
-  </si>
-  <si>
-    <t>maths</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>testuser4@plancess.com</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>testuser5@plancess.com</t>
-  </si>
-  <si>
-    <t>testuser6@plancess.com</t>
-  </si>
-  <si>
-    <t>chhaganlal.m@plancess.com</t>
-  </si>
-  <si>
-    <t>chemistry</t>
-  </si>
-  <si>
-    <t>nonexistingemail@plancess.com</t>
-  </si>
-  <si>
-    <t>InvalidPassword</t>
-  </si>
-  <si>
-    <t>http://dev.plancess.com/ui/app/</t>
-  </si>
-  <si>
-    <t>cl100@mailinator.com</t>
-  </si>
-  <si>
-    <t>confirm_password</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>testuser1@mailinator.com</t>
-  </si>
-  <si>
-    <t>web.test.f.l1</t>
-  </si>
-  <si>
-    <t>@mailinator.com</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>9876543210</t>
-  </si>
-  <si>
-    <t>webtestuser2</t>
-  </si>
-  <si>
-    <t>webtestuser3</t>
-  </si>
-  <si>
-    <t>firstname+ltest4</t>
-  </si>
-  <si>
-    <t>firstname.ltest5</t>
-  </si>
-  <si>
-    <t>firstname.ltest6</t>
-  </si>
-  <si>
-    <t>firstname.l7</t>
-  </si>
-  <si>
-    <t>1234567890w8</t>
-  </si>
-  <si>
-    <t>firstname.ltest39</t>
-  </si>
-  <si>
-    <t>emailwebtest11</t>
-  </si>
-  <si>
-    <t>Firstname-ltest12</t>
-  </si>
-  <si>
-    <t>fbEmail</t>
-  </si>
-  <si>
-    <t>fbPassword</t>
-  </si>
-  <si>
-    <t>http://dev.plancess.com/ui/</t>
-  </si>
-  <si>
-    <t>Pla@12345</t>
-  </si>
-  <si>
-    <t>googleEmail</t>
-  </si>
-  <si>
-    <t>googlePassword</t>
-  </si>
-  <si>
-    <t>9167360969</t>
-  </si>
-  <si>
-    <t>ExamType</t>
-  </si>
-  <si>
-    <t>TestDuration</t>
-  </si>
-  <si>
-    <t>DifficultyLevel</t>
-  </si>
-  <si>
-    <t>Physics&gt;Mechanics&gt;Motion In A Plane</t>
-  </si>
-  <si>
-    <t>Main</t>
-  </si>
-  <si>
-    <t>30 mins</t>
-  </si>
-  <si>
-    <t>Easy</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
@@ -448,9 +433,6 @@
   </si>
   <si>
     <t>00: 60: 00</t>
-  </si>
-  <si>
-    <t>30</t>
   </si>
   <si>
     <t>Physics&gt;Waves and Thermodynamics&gt;</t>
@@ -586,12 +568,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -674,7 +656,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="2" sqref="C3 D12 D32"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -762,7 +744,7 @@
   <dimension ref="1:12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="2" sqref="C3 D12 F12"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -787,7 +769,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>19</v>
@@ -796,13 +778,13 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -818,8 +800,8 @@
       <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>98</v>
+      <c r="C2" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -828,19 +810,19 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,8 +832,8 @@
       <c r="B3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>98</v>
+      <c r="C3" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -860,19 +842,19 @@
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -882,29 +864,29 @@
       <c r="B4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,8 +896,8 @@
       <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>98</v>
+      <c r="C5" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
@@ -924,19 +906,19 @@
         <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,8 +928,8 @@
       <c r="B6" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>98</v>
+      <c r="C6" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
@@ -956,19 +938,19 @@
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,8 +960,8 @@
       <c r="B7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>98</v>
+      <c r="C7" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -988,19 +970,19 @@
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,8 +992,8 @@
       <c r="B8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>98</v>
+      <c r="C8" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
@@ -1020,19 +1002,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1042,8 +1024,8 @@
       <c r="B9" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>98</v>
+      <c r="C9" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>11</v>
@@ -1052,19 +1034,19 @@
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1074,8 +1056,8 @@
       <c r="B10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>98</v>
+      <c r="C10" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>11</v>
@@ -1084,19 +1066,19 @@
         <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,8 +1088,8 @@
       <c r="B11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>98</v>
+      <c r="C11" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>11</v>
@@ -1116,19 +1098,19 @@
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1138,8 +1120,8 @@
       <c r="B12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>98</v>
+      <c r="C12" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>11</v>
@@ -1148,19 +1130,19 @@
         <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1205,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3 D12"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1258,10 +1240,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -1296,7 +1278,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3 D12"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1316,10 +1298,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -1331,13 +1313,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>89</v>
+        <v>109</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1370,7 +1352,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="2" sqref="C3 D12 F14"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1390,10 +1372,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
@@ -1408,16 +1390,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>89</v>
+        <v>109</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1450,7 +1432,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="C3 D12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1483,13 +1465,13 @@
         <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>72</v>
@@ -1506,34 +1488,34 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1541,34 +1523,34 @@
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>132</v>
+      <c r="J3" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,34 +1558,34 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G4" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="I4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>132</v>
+        <v>78</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1611,34 +1593,34 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>139</v>
+        <v>78</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1646,34 +1628,34 @@
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>132</v>
+        <v>81</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1681,34 +1663,34 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>139</v>
+      <c r="J7" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1716,34 +1698,34 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>139</v>
+        <v>78</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1794,7 +1776,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="2" sqref="C3 D12 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1945,7 +1927,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="C3 D12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2158,10 +2140,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="2" sqref="C3 D12 H7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2205,12 +2187,12 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -2222,139 +2204,24 @@
       <c r="F2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="0" t="s">
         <v>79</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
-    <hyperlink ref="B3" r:id="rId3" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C3" r:id="rId4" display="testuser2@plancess.com"/>
-    <hyperlink ref="D3" r:id="rId5" display="P@ssw0rd"/>
-    <hyperlink ref="B4" r:id="rId6" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C4" r:id="rId7" display="testuser4@plancess.com"/>
-    <hyperlink ref="D4" r:id="rId8" display="P@ssw0rd"/>
-    <hyperlink ref="B5" r:id="rId9" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C5" r:id="rId10" display="testuser5@plancess.com"/>
-    <hyperlink ref="D5" r:id="rId11" display="P@ssw0rd"/>
-    <hyperlink ref="B6" r:id="rId12" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C6" r:id="rId13" display="testuser6@plancess.com"/>
-    <hyperlink ref="D6" r:id="rId14" display="P@ssw0rd"/>
+    <hyperlink ref="C2" r:id="rId2" display="chhaganlal.m@plancess.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2373,8 +2240,8 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="C3 D12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2416,16 +2283,16 @@
         <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2436,13 +2303,13 @@
         <v>75</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>83</v>
@@ -2481,7 +2348,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="2" sqref="C3 D12 B18"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2518,8 +2385,8 @@
       <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>91</v>
+      <c r="C2" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -2555,7 +2422,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="2" sqref="C3 D12 C18"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2592,11 +2459,11 @@
       <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>76</v>
+      <c r="C2" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2628,7 +2495,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3 D12"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2663,10 +2530,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -2701,7 +2568,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="2" sqref="C3 D12 B19"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2738,8 +2605,8 @@
       <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>76</v>
+      <c r="C2" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
added user profile test
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,13 +22,14 @@
     <sheet name="loginWithFacebook" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="loginWithGoogle" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="createAssessment" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="userProfile" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="145">
   <si>
     <t>Flag</t>
   </si>
@@ -442,18 +443,40 @@
   </si>
   <si>
     <t>Physics&gt;Modern Physics&gt;Modern Physics,Chemistry&gt;Physical Chemistry&gt;Atomic Structure,Mathematics&gt;Trigonometry&gt;Solutions of Triangle</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>profilePic</t>
+  </si>
+  <si>
+    <t>emailNotification</t>
+  </si>
+  <si>
+    <t>filePath</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>pic.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -492,6 +515,14 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -539,7 +570,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -573,6 +604,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -655,7 +694,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -743,7 +782,7 @@
   </sheetPr>
   <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -1204,7 +1243,7 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1277,7 +1316,7 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1351,7 +1390,7 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1431,8 +1470,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1768,6 +1807,122 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="10" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="10" t="n">
+        <v>33113</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2 J2:K2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
+    <hyperlink ref="C2" r:id="rId2" display="stestuser1@mailinator.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -1775,7 +1930,7 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1926,7 +2081,7 @@
   </sheetPr>
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2142,7 +2297,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2240,7 +2395,7 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2347,7 +2502,7 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2421,7 +2576,7 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2494,7 +2649,7 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2567,7 +2722,7 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added forgot password scenario
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,13 +22,14 @@
     <sheet name="loginWithFacebook" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="loginWithGoogle" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="createAssessment" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="resetPasswordValid" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="138">
   <si>
     <t>Flag</t>
   </si>
@@ -327,9 +328,6 @@
     <t>webtestuser3</t>
   </si>
   <si>
-    <t>firstname+ltest4</t>
-  </si>
-  <si>
     <t>firstname.ltest5</t>
   </si>
   <si>
@@ -442,6 +440,9 @@
   </si>
   <si>
     <t>Physics&gt;Modern Physics&gt;Modern Physics,Chemistry&gt;Physical Chemistry&gt;Atomic Structure,Mathematics&gt;Trigonometry&gt;Solutions of Triangle</t>
+  </si>
+  <si>
+    <t>cl140@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -741,10 +742,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:12"/>
+  <dimension ref="1:11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -905,7 +906,7 @@
       <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>99</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1113,41 +1114,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A12" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A11" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1183,9 +1152,6 @@
     <hyperlink ref="B11" r:id="rId28" location="/" display="http://dev.plancess.com/ui/app/#/"/>
     <hyperlink ref="D11" r:id="rId29" display="P@ssw0rd"/>
     <hyperlink ref="E11" r:id="rId30" display="P@ssw0rd"/>
-    <hyperlink ref="B12" r:id="rId31" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D12" r:id="rId32" display="P@ssw0rd"/>
-    <hyperlink ref="E12" r:id="rId33" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1298,10 +1264,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -1313,13 +1279,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1372,10 +1338,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
@@ -1390,16 +1356,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1431,8 +1397,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1465,13 +1431,13 @@
         <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>72</v>
@@ -1488,34 +1454,34 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>121</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>81</v>
       </c>
       <c r="J2" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1523,34 +1489,34 @@
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>127</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>83</v>
       </c>
       <c r="J3" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1558,34 +1524,34 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>131</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>78</v>
       </c>
       <c r="J4" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,25 +1559,25 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="G5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>133</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>134</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>78</v>
@@ -1628,34 +1594,34 @@
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>81</v>
       </c>
       <c r="J6" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,25 +1629,25 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>83</v>
@@ -1698,25 +1664,25 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>78</v>
@@ -1757,6 +1723,79 @@
     <hyperlink ref="B8" r:id="rId19" display="http://dev.plancess.com/ui/"/>
     <hyperlink ref="C8" r:id="rId20" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D8" r:id="rId21" display="P@ssw0rd"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="cl140@mailinator.com"/>
+    <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2495,7 +2534,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Added Mobile No changes
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="150">
   <si>
     <t>Flag</t>
   </si>
@@ -446,6 +446,12 @@
     <t>cl140@mailinator.com</t>
   </si>
   <si>
+    <t>mobile_Country</t>
+  </si>
+  <si>
+    <t>mobile_Country_Code</t>
+  </si>
+  <si>
     <t>dob</t>
   </si>
   <si>
@@ -459,6 +465,34 @@
   </si>
   <si>
     <t>Web</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">India (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">भारत</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t>+91</t>
+  </si>
+  <si>
+    <t>9920543210</t>
   </si>
   <si>
     <t>2018</t>
@@ -476,7 +510,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -518,6 +552,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="FreeSans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -562,7 +601,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -597,6 +636,10 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1423,7 +1466,7 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -1838,19 +1881,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3826530612245"/>
-    <col collapsed="false" hidden="false" max="10" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1873,23 +1919,29 @@
         <v>91</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -1905,33 +1957,39 @@
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2" s="9" t="n">
+      <c r="G2" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="J2" s="10" t="n">
         <v>33113</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>144</v>
+      <c r="K2" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2 J2:K2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2 L2:M2" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Updated Mobile No and Birthdate selection changes
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="159">
   <si>
     <t>Flag</t>
   </si>
@@ -475,6 +475,7 @@
         <sz val="10"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">भारत</t>
     </r>
@@ -495,10 +496,56 @@
     <t>9920543210</t>
   </si>
   <si>
-    <t>2018</t>
+    <t>01/10/1992</t>
+  </si>
+  <si>
+    <t>2016</t>
   </si>
   <si>
     <t>pic.jpg</t>
+  </si>
+  <si>
+    <t>stestuser2@mailinator.com</t>
+  </si>
+  <si>
+    <t>Web't</t>
+  </si>
+  <si>
+    <t>User't</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Yemen (‫</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">اليمن‬‎</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t>+967</t>
+  </si>
+  <si>
+    <t>711678654</t>
+  </si>
+  <si>
+    <t>30/01/2002</t>
+  </si>
+  <si>
+    <t>2021</t>
   </si>
 </sst>
 </file>
@@ -510,7 +557,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -552,6 +599,18 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="FreeSans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -601,7 +660,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -643,6 +702,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1881,22 +1944,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.4183673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,11 +2038,11 @@
       <c r="I2" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="J2" s="10" t="n">
-        <v>33113</v>
+      <c r="J2" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>7</v>
@@ -1984,12 +2051,56 @@
         <v>7</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2 L2:M2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A3 L2:M3" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1998,6 +2109,9 @@
     <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
     <hyperlink ref="C2" r:id="rId2" display="stestuser1@mailinator.com"/>
     <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+    <hyperlink ref="B3" r:id="rId4" display="http://dev.plancess.com/ui/"/>
+    <hyperlink ref="C3" r:id="rId5" display="stestuser2@mailinator.com"/>
+    <hyperlink ref="D3" r:id="rId6" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
updated test as per new ui changes
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -434,7 +434,7 @@
     <t>Extreme</t>
   </si>
   <si>
-    <t>Physics&gt;Waves and Thermodynamics&gt;</t>
+    <t>Physics&gt;Optics&gt;</t>
   </si>
   <si>
     <t>Physics&gt;Waves and Thermodynamics&gt;,Chemistry&gt;Inorganic Chemistry&gt;</t>
@@ -522,6 +522,7 @@
         <sz val="10"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">اليمن‬‎</t>
     </r>
@@ -557,7 +558,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -606,17 +607,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -660,7 +650,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -702,10 +692,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1529,8 +1515,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1946,7 +1932,7 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -2058,10 +2044,10 @@
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="4" t="s">
         <v>151</v>
       </c>
       <c r="D3" s="4" t="s">

</xml_diff>

<commit_message>
to make remaining tests stable
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -1516,7 +1516,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1674,7 +1674,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>108</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
to run smoke tests on jenkins
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="160">
   <si>
     <t>Flag</t>
   </si>
@@ -260,24 +260,30 @@
     <t>http://dev.plancess.com/ui/app/#/</t>
   </si>
   <si>
+    <t>clmathuriya@gmail.com</t>
+  </si>
+  <si>
+    <t>chemistry</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>01: 00: 00</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
     <t>chhaganlal.m@plancess.com</t>
   </si>
   <si>
-    <t>chemistry</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>01: 00: 00</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
+    <t>webuser1446445200108@mailinator.com</t>
+  </si>
+  <si>
     <t>physics</t>
   </si>
   <si>
@@ -296,9 +302,6 @@
     <t>http://dev.plancess.com/ui/app/</t>
   </si>
   <si>
-    <t>cl100@mailinator.com</t>
-  </si>
-  <si>
     <t>confirm_password</t>
   </si>
   <si>
@@ -380,88 +383,88 @@
     <t>DifficultyLevel</t>
   </si>
   <si>
+    <t>Physics&gt;Mechanics&gt;Motion In A Plane</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>30 mins</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>00: 30: 00</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Physics&gt;Optics&gt;Wave Optics,Chemistry&gt;Organic Chemistry&gt;Alkanes,Mathematics&gt;Vectors &amp; 3D&gt;3D Geometry</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>45 mins</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>00: 45: 00</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Mathematics&gt;Calculus&gt;Differential Equations,Mathematics&gt;Calculus&gt;Definite Integration,Mathematics&gt;Calculus&gt;Indefinite Integration,Mathematics&gt;Calculus&gt;Relations and Functions</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>Mathematics&gt;Calculus&gt;Differential Equations,Mathematics&gt;Calculus&gt;Definite Integration,Mathematics&gt;Calculus&gt;Indefinite Integration,Mathematics&gt;Calculus&gt;Relations and Functions,Mathematics&gt;Algebra&gt;Basic Mathematics,Mathematics&gt;Algebra&gt;Binomial Theorem,Mathematics&gt;Algebra&gt;Complex Number,Mathematics&gt;Algebra&gt;Determinants</t>
+  </si>
+  <si>
+    <t>60 mins</t>
+  </si>
+  <si>
+    <t>Extreme</t>
+  </si>
+  <si>
+    <t>Physics&gt;Optics&gt;</t>
+  </si>
+  <si>
+    <t>Physics&gt;Waves and Thermodynamics&gt;,Chemistry&gt;Inorganic Chemistry&gt;</t>
+  </si>
+  <si>
+    <t>Physics&gt;Modern Physics&gt;Modern Physics,Chemistry&gt;Physical Chemistry&gt;Atomic Structure,Mathematics&gt;Trigonometry&gt;Solutions of Triangle</t>
+  </si>
+  <si>
+    <t>cl101@mailinator.com</t>
+  </si>
+  <si>
+    <t>mobile_Country</t>
+  </si>
+  <si>
+    <t>mobile_Country_Code</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>profilePic</t>
+  </si>
+  <si>
+    <t>emailNotification</t>
+  </si>
+  <si>
+    <t>filePath</t>
+  </si>
+  <si>
     <t>stestuser1@mailinator.com</t>
-  </si>
-  <si>
-    <t>Physics&gt;Mechanics&gt;Motion In A Plane</t>
-  </si>
-  <si>
-    <t>Main</t>
-  </si>
-  <si>
-    <t>30 mins</t>
-  </si>
-  <si>
-    <t>Easy</t>
-  </si>
-  <si>
-    <t>00: 30: 00</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Physics&gt;Optics&gt;Wave Optics,Chemistry&gt;Organic Chemistry&gt;Alkanes,Mathematics&gt;Vectors &amp; 3D&gt;3D Geometry</t>
-  </si>
-  <si>
-    <t>Advanced</t>
-  </si>
-  <si>
-    <t>45 mins</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>00: 45: 00</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Mathematics&gt;Calculus&gt;Differential Equations,Mathematics&gt;Calculus&gt;Definite Integration,Mathematics&gt;Calculus&gt;Indefinite Integration,Mathematics&gt;Calculus&gt;Relations and Functions</t>
-  </si>
-  <si>
-    <t>Hard</t>
-  </si>
-  <si>
-    <t>Mathematics&gt;Calculus&gt;Differential Equations,Mathematics&gt;Calculus&gt;Definite Integration,Mathematics&gt;Calculus&gt;Indefinite Integration,Mathematics&gt;Calculus&gt;Relations and Functions,Mathematics&gt;Algebra&gt;Basic Mathematics,Mathematics&gt;Algebra&gt;Binomial Theorem,Mathematics&gt;Algebra&gt;Complex Number,Mathematics&gt;Algebra&gt;Determinants</t>
-  </si>
-  <si>
-    <t>60 mins</t>
-  </si>
-  <si>
-    <t>Extreme</t>
-  </si>
-  <si>
-    <t>Physics&gt;Optics&gt;</t>
-  </si>
-  <si>
-    <t>Physics&gt;Waves and Thermodynamics&gt;,Chemistry&gt;Inorganic Chemistry&gt;</t>
-  </si>
-  <si>
-    <t>Physics&gt;Modern Physics&gt;Modern Physics,Chemistry&gt;Physical Chemistry&gt;Atomic Structure,Mathematics&gt;Trigonometry&gt;Solutions of Triangle</t>
-  </si>
-  <si>
-    <t>cl140@mailinator.com</t>
-  </si>
-  <si>
-    <t>mobile_Country</t>
-  </si>
-  <si>
-    <t>mobile_Country_Code</t>
-  </si>
-  <si>
-    <t>dob</t>
-  </si>
-  <si>
-    <t>profilePic</t>
-  </si>
-  <si>
-    <t>emailNotification</t>
-  </si>
-  <si>
-    <t>filePath</t>
   </si>
   <si>
     <t>Web</t>
@@ -558,7 +561,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -597,6 +600,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -650,7 +660,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -681,6 +691,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -888,7 +902,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>19</v>
@@ -897,13 +911,13 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -920,7 +934,7 @@
         <v>75</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -929,19 +943,19 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -952,7 +966,7 @@
         <v>75</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -961,19 +975,19 @@
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -984,7 +998,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
@@ -993,19 +1007,19 @@
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,7 +1030,7 @@
         <v>75</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
@@ -1025,19 +1039,19 @@
         <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1048,7 +1062,7 @@
         <v>75</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
@@ -1057,19 +1071,19 @@
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1080,7 +1094,7 @@
         <v>75</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -1089,19 +1103,19 @@
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,7 +1126,7 @@
         <v>75</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
@@ -1121,19 +1135,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,7 +1158,7 @@
         <v>75</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>11</v>
@@ -1153,19 +1167,19 @@
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1176,7 +1190,7 @@
         <v>75</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>11</v>
@@ -1185,19 +1199,19 @@
         <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1208,7 +1222,7 @@
         <v>75</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>11</v>
@@ -1217,19 +1231,19 @@
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>8</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1288,7 +1302,7 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1324,7 +1338,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>76</v>
@@ -1341,7 +1355,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="chhaganlal.m@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="clmathuriya@gmail.com"/>
     <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1382,10 +1396,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -1397,13 +1411,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1456,10 +1470,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
@@ -1474,16 +1488,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1515,8 +1529,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1549,13 +1563,13 @@
         <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>72</v>
@@ -1572,10 +1586,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -1593,9 +1607,9 @@
         <v>120</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>121</v>
       </c>
       <c r="K2" s="0" t="s">
@@ -1607,10 +1621,10 @@
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -1628,9 +1642,9 @@
         <v>126</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>127</v>
       </c>
       <c r="K3" s="0" t="s">
@@ -1642,10 +1656,10 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
@@ -1665,7 +1679,7 @@
       <c r="I4" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="9" t="s">
         <v>127</v>
       </c>
       <c r="K4" s="0" t="s">
@@ -1677,10 +1691,10 @@
         <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
@@ -1700,7 +1714,7 @@
       <c r="I5" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="9" t="s">
         <v>79</v>
       </c>
       <c r="K5" s="0" t="s">
@@ -1712,10 +1726,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
@@ -1733,9 +1747,9 @@
         <v>120</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="J6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>127</v>
       </c>
       <c r="K6" s="0" t="s">
@@ -1747,10 +1761,10 @@
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -1768,9 +1782,9 @@
         <v>126</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="J7" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>79</v>
       </c>
       <c r="K7" s="0" t="s">
@@ -1782,10 +1796,10 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
@@ -1805,7 +1819,7 @@
       <c r="I8" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="9" t="s">
         <v>79</v>
       </c>
       <c r="K8" s="0" t="s">
@@ -1821,25 +1835,25 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C2" r:id="rId2" display="stestuser1@mailinator.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="clmathuriya@gmail.com"/>
     <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
     <hyperlink ref="B3" r:id="rId4" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C3" r:id="rId5" display="stestuser1@mailinator.com"/>
+    <hyperlink ref="C3" r:id="rId5" display="clmathuriya@gmail.com"/>
     <hyperlink ref="D3" r:id="rId6" display="P@ssw0rd"/>
     <hyperlink ref="B4" r:id="rId7" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C4" r:id="rId8" display="stestuser1@mailinator.com"/>
+    <hyperlink ref="C4" r:id="rId8" display="clmathuriya@gmail.com"/>
     <hyperlink ref="D4" r:id="rId9" display="P@ssw0rd"/>
     <hyperlink ref="B5" r:id="rId10" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C5" r:id="rId11" display="stestuser1@mailinator.com"/>
+    <hyperlink ref="C5" r:id="rId11" display="clmathuriya@gmail.com"/>
     <hyperlink ref="D5" r:id="rId12" display="P@ssw0rd"/>
     <hyperlink ref="B6" r:id="rId13" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C6" r:id="rId14" display="stestuser1@mailinator.com"/>
+    <hyperlink ref="C6" r:id="rId14" display="clmathuriya@gmail.com"/>
     <hyperlink ref="D6" r:id="rId15" display="P@ssw0rd"/>
     <hyperlink ref="B7" r:id="rId16" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C7" r:id="rId17" display="stestuser1@mailinator.com"/>
+    <hyperlink ref="C7" r:id="rId17" display="clmathuriya@gmail.com"/>
     <hyperlink ref="D7" r:id="rId18" display="P@ssw0rd"/>
     <hyperlink ref="B8" r:id="rId19" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C8" r:id="rId20" display="stestuser1@mailinator.com"/>
+    <hyperlink ref="C8" r:id="rId20" display="clmathuriya@gmail.com"/>
     <hyperlink ref="D8" r:id="rId21" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1859,8 +1873,8 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1895,7 +1909,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>137</v>
@@ -1912,7 +1926,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="cl140@mailinator.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="cl101@mailinator.com"/>
     <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1969,7 +1983,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>138</v>
@@ -2001,34 +2015,34 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>145</v>
+        <v>96</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>146</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="J2" s="10" t="s">
         <v>148</v>
       </c>
+      <c r="J2" s="11" t="s">
+        <v>149</v>
+      </c>
       <c r="K2" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>7</v>
@@ -2037,7 +2051,7 @@
         <v>7</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,34 +2059,34 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>7</v>
@@ -2081,7 +2095,7 @@
         <v>22</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2484,7 +2498,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2561,7 +2575,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C2" r:id="rId2" display="chhaganlal.m@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="clmathuriya@gmail.com"/>
     <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2582,7 +2596,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2624,7 +2638,7 @@
         <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -2633,7 +2647,7 @@
         <v>77</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2643,17 +2657,17 @@
       <c r="B3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>76</v>
+      <c r="C3" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2668,8 +2682,7 @@
     <hyperlink ref="C2" r:id="rId2" display="chhaganlal.m@plancess.com"/>
     <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
     <hyperlink ref="B3" r:id="rId4" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C3" r:id="rId5" display="chhaganlal.m@plancess.com"/>
-    <hyperlink ref="D3" r:id="rId6" display="P@ssw0rd"/>
+    <hyperlink ref="D3" r:id="rId5" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2727,7 +2740,7 @@
         <v>75</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -2801,10 +2814,10 @@
         <v>75</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2836,7 +2849,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2871,10 +2884,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -2888,7 +2901,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="cl100@mailinator.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="clmathuriya@gmail.com"/>
     <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2947,7 +2960,7 @@
         <v>75</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
complete test suite for dev.preplane.com
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="157">
   <si>
     <t>Flag</t>
   </si>
@@ -257,9 +257,6 @@
     <t>totalQuestions</t>
   </si>
   <si>
-    <t>http://dev.plancess.com/ui/app/#/</t>
-  </si>
-  <si>
     <t>clmathuriya@gmail.com</t>
   </si>
   <si>
@@ -278,15 +275,15 @@
     <t>chhaganlal.m@plancess.com</t>
   </si>
   <si>
+    <t>physics</t>
+  </si>
+  <si>
     <t>a</t>
   </si>
   <si>
     <t>webuser1446445200108@mailinator.com</t>
   </si>
   <si>
-    <t>physics</t>
-  </si>
-  <si>
     <t>b</t>
   </si>
   <si>
@@ -299,9 +296,6 @@
     <t>InvalidPassword</t>
   </si>
   <si>
-    <t>http://dev.plancess.com/ui/app/</t>
-  </si>
-  <si>
     <t>confirm_password</t>
   </si>
   <si>
@@ -357,9 +351,6 @@
   </si>
   <si>
     <t>fbPassword</t>
-  </si>
-  <si>
-    <t>http://dev.plancess.com/ui/</t>
   </si>
   <si>
     <t>Pla@12345</t>
@@ -876,19 +867,18 @@
   </sheetPr>
   <dimension ref="1:11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,32 +886,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
@@ -930,320 +918,290 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1254,36 +1212,26 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
+    <hyperlink ref="C2" r:id="rId1" display="P@ssw0rd"/>
     <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
-    <hyperlink ref="E2" r:id="rId3" display="P@ssw0rd"/>
-    <hyperlink ref="B3" r:id="rId4" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D3" r:id="rId5" display="P@ssw0rd"/>
-    <hyperlink ref="E3" r:id="rId6" display="P@ssw0rd"/>
-    <hyperlink ref="B4" r:id="rId7" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D4" r:id="rId8" display="P@ssw0rd"/>
-    <hyperlink ref="E4" r:id="rId9" display="P@ssw0rd"/>
-    <hyperlink ref="B5" r:id="rId10" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D5" r:id="rId11" display="P@ssw0rd"/>
-    <hyperlink ref="E5" r:id="rId12" display="P@ssw0rd"/>
-    <hyperlink ref="B6" r:id="rId13" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D6" r:id="rId14" display="P@ssw0rd"/>
-    <hyperlink ref="E6" r:id="rId15" display="P@ssw0rd"/>
-    <hyperlink ref="B7" r:id="rId16" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D7" r:id="rId17" display="P@ssw0rd"/>
-    <hyperlink ref="E7" r:id="rId18" display="P@ssw0rd"/>
-    <hyperlink ref="B8" r:id="rId19" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D8" r:id="rId20" display="P@ssw0rd"/>
-    <hyperlink ref="E8" r:id="rId21" display="P@ssw0rd"/>
-    <hyperlink ref="B9" r:id="rId22" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D9" r:id="rId23" display="P@ssw0rd"/>
-    <hyperlink ref="E9" r:id="rId24" display="P@ssw0rd"/>
-    <hyperlink ref="B10" r:id="rId25" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D10" r:id="rId26" display="P@ssw0rd"/>
-    <hyperlink ref="E10" r:id="rId27" display="P@ssw0rd"/>
-    <hyperlink ref="B11" r:id="rId28" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D11" r:id="rId29" display="P@ssw0rd"/>
-    <hyperlink ref="E11" r:id="rId30" display="P@ssw0rd"/>
+    <hyperlink ref="C3" r:id="rId3" display="P@ssw0rd"/>
+    <hyperlink ref="D3" r:id="rId4" display="P@ssw0rd"/>
+    <hyperlink ref="C4" r:id="rId5" display="P@ssw0rd"/>
+    <hyperlink ref="D4" r:id="rId6" display="P@ssw0rd"/>
+    <hyperlink ref="C5" r:id="rId7" display="P@ssw0rd"/>
+    <hyperlink ref="D5" r:id="rId8" display="P@ssw0rd"/>
+    <hyperlink ref="C6" r:id="rId9" display="P@ssw0rd"/>
+    <hyperlink ref="D6" r:id="rId10" display="P@ssw0rd"/>
+    <hyperlink ref="C7" r:id="rId11" display="P@ssw0rd"/>
+    <hyperlink ref="D7" r:id="rId12" display="P@ssw0rd"/>
+    <hyperlink ref="C8" r:id="rId13" display="P@ssw0rd"/>
+    <hyperlink ref="D8" r:id="rId14" display="P@ssw0rd"/>
+    <hyperlink ref="C9" r:id="rId15" display="P@ssw0rd"/>
+    <hyperlink ref="D9" r:id="rId16" display="P@ssw0rd"/>
+    <hyperlink ref="C10" r:id="rId17" display="P@ssw0rd"/>
+    <hyperlink ref="D10" r:id="rId18" display="P@ssw0rd"/>
+    <hyperlink ref="C11" r:id="rId19" display="P@ssw0rd"/>
+    <hyperlink ref="D11" r:id="rId20" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1303,16 +1251,15 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1320,14 +1267,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -1337,13 +1282,10 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1355,8 +1297,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="clmathuriya@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
+    <hyperlink ref="B2" r:id="rId1" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1376,16 +1318,15 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1393,14 +1334,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -1410,14 +1349,11 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>110</v>
+      <c r="B2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1428,9 +1364,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C2" r:id="rId2" display="chhaganlal.m@plancess.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="Pla@12345"/>
+    <hyperlink ref="B2" r:id="rId1" display="chhaganlal.m@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="Pla@12345"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1450,16 +1385,15 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1467,17 +1401,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -1487,17 +1419,14 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1508,9 +1437,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C2" r:id="rId2" display="chhaganlal.m@plancess.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="Pla@12345"/>
+    <hyperlink ref="B2" r:id="rId1" display="chhaganlal.m@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="Pla@12345"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1527,23 +1455,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="123.515306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="123.515306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,33 +1478,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1586,34 +1510,31 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>114</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="H2" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1621,34 +1542,31 @@
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="H3" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,34 +1574,31 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>126</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G4" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1691,34 +1606,31 @@
         <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>128</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="I5" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,34 +1638,31 @@
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>131</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G6" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="J6" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1761,34 +1670,31 @@
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="J7" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1796,34 +1702,31 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>133</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="I8" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1834,27 +1737,20 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C2" r:id="rId2" display="clmathuriya@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
-    <hyperlink ref="B3" r:id="rId4" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C3" r:id="rId5" display="clmathuriya@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId6" display="P@ssw0rd"/>
-    <hyperlink ref="B4" r:id="rId7" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C4" r:id="rId8" display="clmathuriya@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId9" display="P@ssw0rd"/>
-    <hyperlink ref="B5" r:id="rId10" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C5" r:id="rId11" display="clmathuriya@gmail.com"/>
-    <hyperlink ref="D5" r:id="rId12" display="P@ssw0rd"/>
-    <hyperlink ref="B6" r:id="rId13" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C6" r:id="rId14" display="clmathuriya@gmail.com"/>
-    <hyperlink ref="D6" r:id="rId15" display="P@ssw0rd"/>
-    <hyperlink ref="B7" r:id="rId16" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C7" r:id="rId17" display="clmathuriya@gmail.com"/>
-    <hyperlink ref="D7" r:id="rId18" display="P@ssw0rd"/>
-    <hyperlink ref="B8" r:id="rId19" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C8" r:id="rId20" display="clmathuriya@gmail.com"/>
-    <hyperlink ref="D8" r:id="rId21" display="P@ssw0rd"/>
+    <hyperlink ref="B2" r:id="rId1" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
+    <hyperlink ref="B3" r:id="rId3" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="C3" r:id="rId4" display="P@ssw0rd"/>
+    <hyperlink ref="B4" r:id="rId5" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId6" display="P@ssw0rd"/>
+    <hyperlink ref="B5" r:id="rId7" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="C5" r:id="rId8" display="P@ssw0rd"/>
+    <hyperlink ref="B6" r:id="rId9" display="chhaganlal.m@plancess.com"/>
+    <hyperlink ref="C6" r:id="rId10" display="P@ssw0rd"/>
+    <hyperlink ref="B7" r:id="rId11" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="C7" r:id="rId12" display="P@ssw0rd"/>
+    <hyperlink ref="B8" r:id="rId13" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="C8" r:id="rId14" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1873,16 +1769,15 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,14 +1785,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -1908,13 +1801,10 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1926,8 +1816,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="cl101@mailinator.com"/>
-    <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
+    <hyperlink ref="B2" r:id="rId1" display="cl101@mailinator.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1944,26 +1834,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.9285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.8877551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.8367346938776"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,87 +1860,82 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>143</v>
-      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="10" t="s">
+      <c r="I2" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="K2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2059,59 +1943,54 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>159</v>
+      <c r="K3" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>151</v>
+      <c r="M3" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A3 L2:M3" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A3 K2:L3" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C2" r:id="rId2" display="stestuser1@mailinator.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
-    <hyperlink ref="B3" r:id="rId4" display="http://dev.plancess.com/ui/"/>
-    <hyperlink ref="C3" r:id="rId5" display="stestuser2@mailinator.com"/>
-    <hyperlink ref="D3" r:id="rId6" display="P@ssw0rd"/>
+    <hyperlink ref="B2" r:id="rId1" display="stestuser1@mailinator.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
+    <hyperlink ref="B3" r:id="rId3" display="stestuser2@mailinator.com"/>
+    <hyperlink ref="C3" r:id="rId4" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2495,23 +2374,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3520408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1020408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3520408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2519,39 +2397,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>77</v>
@@ -2561,9 +2437,6 @@
       </c>
       <c r="G2" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2574,9 +2447,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C2" r:id="rId2" display="clmathuriya@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+    <hyperlink ref="B2" r:id="rId1" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2593,21 +2465,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2615,59 +2486,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="0" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>81</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2678,11 +2541,9 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C2" r:id="rId2" display="chhaganlal.m@plancess.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
-    <hyperlink ref="B3" r:id="rId4" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="D3" r:id="rId5" display="P@ssw0rd"/>
+    <hyperlink ref="B2" r:id="rId1" display="chhaganlal.m@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
+    <hyperlink ref="C3" r:id="rId3" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2702,16 +2563,15 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2719,14 +2579,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -2736,13 +2594,10 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2754,9 +2609,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C2" r:id="rId2" display="nonexistingemail@plancess.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+    <hyperlink ref="B2" r:id="rId1" display="nonexistingemail@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2776,16 +2630,15 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2793,14 +2646,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -2810,14 +2661,11 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2828,8 +2676,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="testuser1@plancess.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2849,16 +2696,15 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2866,14 +2712,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -2883,13 +2727,10 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2901,8 +2742,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="clmathuriya@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId2" display="P@ssw0rd"/>
+    <hyperlink ref="B2" r:id="rId1" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2922,16 +2763,15 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2939,14 +2779,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
@@ -2956,13 +2794,10 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2974,9 +2809,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="/" display="http://dev.plancess.com/ui/app/#/"/>
-    <hyperlink ref="C2" r:id="rId2" display="testuser1@plancess.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="P@ssw0rd"/>
+    <hyperlink ref="B2" r:id="rId1" display="testuser1@plancess.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added Login Test for plancess website
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,13 +24,14 @@
     <sheet name="createAssessment" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="resetPasswordValid" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="userProfile" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="PlancessUserData" sheetId="17" state="visible" r:id="rId18"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="163">
   <si>
     <t>Flag</t>
   </si>
@@ -522,6 +523,7 @@
         <sz val="10"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">اليمن‬‎</t>
     </r>
@@ -547,6 +549,18 @@
   <si>
     <t>2021</t>
   </si>
+  <si>
+    <t>saumen</t>
+  </si>
+  <si>
+    <t>saumen.d@plancess.com</t>
+  </si>
+  <si>
+    <t>plancess</t>
+  </si>
+  <si>
+    <t>http://dev.plancess.com/</t>
+  </si>
 </sst>
 </file>
 
@@ -557,7 +571,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -606,17 +620,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -660,7 +663,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -702,10 +705,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1946,8 +1945,8 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2058,10 +2057,10 @@
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="4" t="s">
         <v>151</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2123,6 +2122,84 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="saumen.d@plancess.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -2130,8 +2207,8 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
updated tests for preplane.com
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="892" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="892" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="159">
   <si>
     <t>Flag</t>
   </si>
@@ -258,45 +258,48 @@
     <t>totalQuestions</t>
   </si>
   <si>
+    <t>makarand.d@plancess.com</t>
+  </si>
+  <si>
+    <t>mathematics</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>01: 00: 00</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>chhaganlal.m@plancess.com</t>
+  </si>
+  <si>
+    <t>physics</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>webuser1446445200108@mailinator.com</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>nonexistingemail@plancess.com</t>
+  </si>
+  <si>
+    <t>testuser1@plancess.com</t>
+  </si>
+  <si>
+    <t>InvalidPassword</t>
+  </si>
+  <si>
     <t>clmathuriya@gmail.com</t>
   </si>
   <si>
-    <t>chemistry</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>01: 00: 00</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>chhaganlal.m@plancess.com</t>
-  </si>
-  <si>
-    <t>physics</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>webuser1446445200108@mailinator.com</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>nonexistingemail@plancess.com</t>
-  </si>
-  <si>
-    <t>testuser1@plancess.com</t>
-  </si>
-  <si>
-    <t>InvalidPassword</t>
-  </si>
-  <si>
     <t>confirm_password</t>
   </si>
   <si>
@@ -454,9 +457,6 @@
   </si>
   <si>
     <t>filePath</t>
-  </si>
-  <si>
-    <t>stestuser1@mailinator.com</t>
   </si>
   <si>
     <t>Web</t>
@@ -498,9 +498,6 @@
   </si>
   <si>
     <t>pic.jpg</t>
-  </si>
-  <si>
-    <t>stestuser2@mailinator.com</t>
   </si>
   <si>
     <t>Web't</t>
@@ -899,7 +896,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
@@ -908,13 +905,13 @@
         <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
@@ -929,7 +926,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -938,19 +935,19 @@
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,7 +955,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
@@ -967,19 +964,19 @@
         <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -987,7 +984,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
@@ -996,19 +993,19 @@
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,7 +1013,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
@@ -1025,19 +1022,19 @@
         <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1045,7 +1042,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
@@ -1054,19 +1051,19 @@
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1074,7 +1071,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
@@ -1083,19 +1080,19 @@
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,7 +1100,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>11</v>
@@ -1112,19 +1109,19 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,7 +1129,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>11</v>
@@ -1141,19 +1138,19 @@
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1161,7 +1158,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>11</v>
@@ -1170,19 +1167,19 @@
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,7 +1187,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>11</v>
@@ -1199,19 +1196,19 @@
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1293,7 +1290,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -1344,10 +1341,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -1363,7 +1360,7 @@
         <v>80</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1411,10 +1408,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
@@ -1433,10 +1430,10 @@
         <v>80</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1497,13 +1494,13 @@
         <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>72</v>
@@ -1520,31 +1517,31 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>82</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,31 +1549,31 @@
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>84</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1584,31 +1581,31 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,22 +1613,22 @@
         <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>77</v>
@@ -1654,25 +1651,25 @@
         <v>11</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>82</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,22 +1677,22 @@
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>84</v>
@@ -1712,22 +1709,22 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>77</v>
@@ -1812,7 +1809,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -1846,8 +1843,8 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1879,31 +1876,31 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -1912,7 +1909,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -1921,7 +1918,7 @@
         <v>142</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>143</v>
@@ -1953,31 +1950,31 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>156</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>7</v>
@@ -1997,9 +1994,9 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="stestuser1@mailinator.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="chhaganlal.m@plancess.com"/>
     <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
-    <hyperlink ref="B3" r:id="rId3" display="stestuser2@mailinator.com"/>
+    <hyperlink ref="B3" r:id="rId3" display="chhaganlal.m@plancess.com"/>
     <hyperlink ref="C3" r:id="rId4" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2019,7 +2016,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -2049,13 +2046,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2453,7 +2450,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2523,7 +2520,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="makarand.d@plancess.com"/>
     <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2804,7 +2801,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
updated test to make build stable
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -1844,7 +1844,7 @@
   <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
changes in userprofile test
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="892" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="892" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -1846,8 +1846,8 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>141</v>
@@ -2019,7 +2019,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
excluded create test to avoid no more questions available problem
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,33 +5,33 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="892" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="892" firstSheet="3" activeTab="15"/>
   </bookViews>
   <sheets>
-    <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="lmsUserData" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Campaign" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="signup" sheetId="1" state="hidden" r:id="rId2"/>
+    <sheet name="lmsUserData" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Campaign" sheetId="3" state="hidden" r:id="rId4"/>
     <sheet name="assessment_valid" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="assessment_no_test" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="nonExistingEmails" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="invalidPasswords" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="loginWithValidEmailPassword" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="signupInvalidEmails" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="signUpvalidEmailPasswords" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="signupInvalidEmails" sheetId="9" state="hidden" r:id="rId10"/>
+    <sheet name="signUpvalidEmailPasswords" sheetId="10" state="hidden" r:id="rId11"/>
     <sheet name="dashboard" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="loginWithFacebook" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="loginWithGoogle" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="createAssessment" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="resetPasswordValid" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="userProfile" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="PlancessWebsiteUserData" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="PlancessWebsiteUserData" sheetId="17" state="hidden" r:id="rId18"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="157">
   <si>
     <t>Flag</t>
   </si>
@@ -258,7 +258,7 @@
     <t>totalQuestions</t>
   </si>
   <si>
-    <t>makarand.d@plancess.com</t>
+    <t>demo.user@plancess.com</t>
   </si>
   <si>
     <t>mathematics</t>
@@ -297,9 +297,6 @@
     <t>InvalidPassword</t>
   </si>
   <si>
-    <t>clmathuriya@gmail.com</t>
-  </si>
-  <si>
     <t>confirm_password</t>
   </si>
   <si>
@@ -436,9 +433,6 @@
   </si>
   <si>
     <t>Physics&gt;Modern Physics&gt;Modern Physics,Chemistry&gt;Physical Chemistry&gt;Atomic Structure,Mathematics&gt;Trigonometry&gt;Solutions of Triangle</t>
-  </si>
-  <si>
-    <t>cl101@mailinator.com</t>
   </si>
   <si>
     <t>mobile_Country</t>
@@ -896,7 +890,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
@@ -905,13 +899,13 @@
         <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>14</v>
@@ -926,28 +920,28 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -955,7 +949,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
@@ -964,19 +958,19 @@
         <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -984,7 +978,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
@@ -993,19 +987,19 @@
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,7 +1007,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
@@ -1022,19 +1016,19 @@
         <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1042,7 +1036,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
@@ -1051,19 +1045,19 @@
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1071,7 +1065,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
@@ -1080,19 +1074,19 @@
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,7 +1094,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>11</v>
@@ -1109,19 +1103,19 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,7 +1123,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>11</v>
@@ -1138,19 +1132,19 @@
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H9" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,7 +1152,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>11</v>
@@ -1167,19 +1161,19 @@
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1187,7 +1181,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>11</v>
@@ -1196,19 +1190,19 @@
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1252,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1290,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -1304,7 +1298,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="demo.user@plancess.com"/>
     <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1325,7 +1319,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1341,10 +1335,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -1360,7 +1354,7 @@
         <v>80</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1408,10 +1402,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
@@ -1430,10 +1424,10 @@
         <v>80</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1464,7 +1458,7 @@
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1494,13 +1488,13 @@
         <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>72</v>
@@ -1517,31 +1511,31 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>118</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>82</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,31 +1543,31 @@
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>124</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>84</v>
       </c>
       <c r="I3" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1581,31 +1575,31 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>127</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>128</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,22 +1607,22 @@
         <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>131</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>77</v>
@@ -1645,31 +1639,31 @@
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>82</v>
       </c>
       <c r="I6" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="J6" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1677,22 +1671,22 @@
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>84</v>
@@ -1709,22 +1703,22 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>77</v>
@@ -1744,19 +1738,19 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="demo.user@plancess.com"/>
     <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
-    <hyperlink ref="B3" r:id="rId3" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId3" display="demo.user@plancess.com"/>
     <hyperlink ref="C3" r:id="rId4" display="P@ssw0rd"/>
-    <hyperlink ref="B4" r:id="rId5" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId5" display="demo.user@plancess.com"/>
     <hyperlink ref="C4" r:id="rId6" display="P@ssw0rd"/>
-    <hyperlink ref="B5" r:id="rId7" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId7" display="demo.user@plancess.com"/>
     <hyperlink ref="C5" r:id="rId8" display="P@ssw0rd"/>
-    <hyperlink ref="B6" r:id="rId9" display="chhaganlal.m@plancess.com"/>
+    <hyperlink ref="B6" r:id="rId9" display="demo.user@plancess.com"/>
     <hyperlink ref="C6" r:id="rId10" display="P@ssw0rd"/>
-    <hyperlink ref="B7" r:id="rId11" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="B7" r:id="rId11" display="demo.user@plancess.com"/>
     <hyperlink ref="C7" r:id="rId12" display="P@ssw0rd"/>
-    <hyperlink ref="B8" r:id="rId13" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="B8" r:id="rId13" display="demo.user@plancess.com"/>
     <hyperlink ref="C8" r:id="rId14" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1777,7 +1771,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1808,8 +1802,8 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>135</v>
+      <c r="B2" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -1823,7 +1817,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="cl101@mailinator.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="demo.user@plancess.com"/>
     <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1844,7 +1838,7 @@
   <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1876,31 +1870,31 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -1908,41 +1902,41 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>80</v>
+      <c r="B2" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="H2" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="I2" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="K2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,25 +1950,25 @@
         <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>153</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>155</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>7</v>
@@ -1983,7 +1977,7 @@
         <v>22</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1994,7 +1988,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="chhaganlal.m@plancess.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="demo.user@plancess.com"/>
     <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
     <hyperlink ref="B3" r:id="rId3" display="chhaganlal.m@plancess.com"/>
     <hyperlink ref="C3" r:id="rId4" display="P@ssw0rd"/>
@@ -2017,7 +2011,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2046,13 +2040,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2450,7 +2444,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2520,7 +2514,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="makarand.d@plancess.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="demo.user@plancess.com"/>
     <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2769,7 +2763,7 @@
   <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2801,7 +2795,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -2815,7 +2809,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="clmathuriya@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="demo.user@plancess.com"/>
     <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
modified test cases as per latest changes in ui
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -1477,7 +1477,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>91</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
updated some tests as per latest ui
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -420,7 +420,7 @@
     <t>20</t>
   </si>
   <si>
-    <t>Mathematics&gt;Calculus&gt;Differential Equations,Mathematics&gt;Calculus&gt;Definite Integration,Mathematics&gt;Calculus&gt;Indefinite Integration,Mathematics&gt;Calculus&gt;Relations and Functions</t>
+    <t>Mathematics&gt;Calculus&gt;Differential Equations</t>
   </si>
   <si>
     <t>Hard</t>
@@ -1477,7 +1477,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>91</v>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
modified dashboard, take test
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="892" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="892" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="164">
   <si>
     <t>Flag</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>webuser1453380325316@mailinator.com</t>
   </si>
   <si>
     <t>nonexistingemail@plancess.com</t>
@@ -707,12 +710,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -908,7 +911,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
@@ -917,7 +920,7 @@
         <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -938,7 +941,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -947,10 +950,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>8</v>
@@ -959,7 +962,7 @@
         <v>78</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,7 +970,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
@@ -976,10 +979,10 @@
         <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>8</v>
@@ -988,7 +991,7 @@
         <v>78</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -996,7 +999,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
@@ -1005,10 +1008,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>8</v>
@@ -1017,7 +1020,7 @@
         <v>78</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,7 +1028,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
@@ -1034,10 +1037,10 @@
         <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>8</v>
@@ -1046,7 +1049,7 @@
         <v>78</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1054,7 +1057,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
@@ -1063,10 +1066,10 @@
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>8</v>
@@ -1075,7 +1078,7 @@
         <v>78</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,7 +1086,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
@@ -1092,10 +1095,10 @@
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>8</v>
@@ -1104,7 +1107,7 @@
         <v>78</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,7 +1115,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>11</v>
@@ -1121,10 +1124,10 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>8</v>
@@ -1133,7 +1136,7 @@
         <v>78</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1141,7 +1144,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>11</v>
@@ -1150,10 +1153,10 @@
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>8</v>
@@ -1162,7 +1165,7 @@
         <v>78</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,7 +1173,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>11</v>
@@ -1179,10 +1182,10 @@
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>8</v>
@@ -1191,7 +1194,7 @@
         <v>78</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,7 +1202,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>11</v>
@@ -1208,10 +1211,10 @@
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>8</v>
@@ -1220,7 +1223,7 @@
         <v>78</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1302,7 +1305,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -1353,10 +1356,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -1369,10 +1372,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1420,10 +1423,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
@@ -1439,13 +1442,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1476,7 +1479,7 @@
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1506,13 +1509,13 @@
         <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>73</v>
@@ -1529,31 +1532,31 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>121</v>
+      <c r="I2" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1561,31 +1564,31 @@
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>127</v>
+      <c r="I3" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,31 +1596,31 @@
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>127</v>
+      <c r="I4" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,27 +1628,27 @@
         <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="10" t="s">
         <v>81</v>
       </c>
       <c r="J5" s="0" t="s">
@@ -1657,31 +1660,31 @@
         <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>127</v>
+      <c r="I6" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,27 +1692,27 @@
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="10" t="s">
         <v>81</v>
       </c>
       <c r="J7" s="0" t="s">
@@ -1721,27 +1724,27 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="10" t="s">
         <v>81</v>
       </c>
       <c r="J8" s="0" t="s">
@@ -1821,7 +1824,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -1891,28 +1894,28 @@
         <v>71</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -1921,31 +1924,31 @@
         <v>22</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>146</v>
+      <c r="F2" s="9" t="s">
+        <v>147</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>7</v>
@@ -1954,7 +1957,7 @@
         <v>7</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,31 +1965,31 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>7</v>
@@ -1995,7 +1998,7 @@
         <v>22</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2058,13 +2061,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2561,10 +2564,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:3"/>
+  <dimension ref="1:4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2597,7 +2600,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>83</v>
@@ -2614,7 +2617,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>86</v>
@@ -2629,16 +2632,35 @@
         <v>87</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A3" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A4" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="P@ssw0rd"/>
-    <hyperlink ref="C3" r:id="rId2" display="P@ssw0rd"/>
+    <hyperlink ref="B2" r:id="rId1" display="webuser1446299916884@mailinator.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="P@ssw0rd"/>
+    <hyperlink ref="C3" r:id="rId3" display="P@ssw0rd"/>
+    <hyperlink ref="C4" r:id="rId4" display="P@ssw0rd"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2690,7 +2712,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -2757,10 +2779,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2823,7 +2845,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -2890,7 +2912,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>

</xml_diff>